<commit_message>
Auto-submit on dropdown selection; added modals and improved assets
- Implemented auto-submit on dropdown menu selection
- Added info, search, email and warning modals
- Commented spreadsheet data validation
- Made JS and CSS links local
</commit_message>
<xml_diff>
--- a/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.1.xlsx
+++ b/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.1.xlsx
@@ -16,18 +16,18 @@
     <sheet name="cell_suspension" sheetId="7" r:id="rId7"/>
     <sheet name="lib_prep" sheetId="8" r:id="rId8"/>
     <sheet name="sequencing" sheetId="9" r:id="rId9"/>
-    <sheet name="file" sheetId="10" r:id="rId10"/>
-    <sheet name="analysis_derived_data" sheetId="11" r:id="rId11"/>
-    <sheet name="raw_data_processing" sheetId="12" r:id="rId12"/>
-    <sheet name="downstream_processing" sheetId="13" r:id="rId13"/>
-    <sheet name="data_availability_checklist" sheetId="14" r:id="rId14"/>
+    <sheet name="analysis_derived_data" sheetId="10" r:id="rId10"/>
+    <sheet name="raw_data_processing" sheetId="11" r:id="rId11"/>
+    <sheet name="downstream_processing" sheetId="12" r:id="rId12"/>
+    <sheet name="data_availability_checklist" sheetId="13" r:id="rId13"/>
+    <sheet name="file" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="789">
   <si>
     <t>key</t>
   </si>
@@ -50,10 +50,10 @@
     <t>version_dwc_sc_rnaseq</t>
   </si>
   <si>
-    <t>Single-cell RNA Sequencing [Darwin Core (DwC)]</t>
-  </si>
-  <si>
-    <t>TBC dwc_sc_rnaseq</t>
+    <t>Single-cell Ribonucleic Acid Sequencing (scRNA-Seq) [Darwin Core (DwC)]</t>
+  </si>
+  <si>
+    <t>A genomic approach for detecting and quantitatively analysing messenger Ribonucleic Acid (RNA) in individual cells, aimed at transmitting biodiversity-related information in alignment with the Darwin Core (DwC) standard.</t>
   </si>
   <si>
     <t>dwc</t>
@@ -98,7 +98,7 @@
     <t>A detailed description of the project which includes research goals and experimental approach. Project description should be fewer than 300 words, such as an abstract from a grant application or publication.</t>
   </si>
   <si>
-    <t>e.g. This project explores the intricate details of single cells in the human body, focusing on their structure, function, and behavior. By studying individual cells, it aims to uncover how they contribute to overall health, disease progression, and human biology. This research can provide deeper insights into cellular processes, paving the way for advancements in medical treatments and personalised medicine.</t>
+    <t>e.g. This project explores the intricate details of single cells in the human body, focusing on their structure, function, and behaviour. By studying individual cells, it aims to uncover how they contribute to overall health, disease progression, and human biology. This research can provide deeper insights into cellular processes, paving the way for advancements in medical treatments and personalised medicine.</t>
   </si>
   <si>
     <t>A citation for the study resource, following a standard format.</t>
@@ -152,12 +152,18 @@
     <t>Spatial Transcriptomics</t>
   </si>
   <si>
+    <t>orcid_id</t>
+  </si>
+  <si>
     <t>givenName</t>
   </si>
   <si>
     <t>familyName</t>
   </si>
   <si>
+    <t>email</t>
+  </si>
+  <si>
     <t>affiliation</t>
   </si>
   <si>
@@ -167,25 +173,43 @@
     <t>funding</t>
   </si>
   <si>
+    <t>orcid_id (optional)</t>
+  </si>
+  <si>
+    <t>email (optional)</t>
+  </si>
+  <si>
     <t>funder (optional)</t>
   </si>
   <si>
     <t>funding (optional)</t>
   </si>
   <si>
-    <t>The first name of a Person.</t>
+    <t>A 16-digit number that uniquely identify researchers.</t>
+  </si>
+  <si>
+    <t>e.g. 0000-1234-5678-9012</t>
+  </si>
+  <si>
+    <t>A first name (or given name) is the personal name given to an individual conducting the study.</t>
   </si>
   <si>
     <t>e.g. Jane</t>
   </si>
   <si>
-    <t>The last name of a Person.</t>
+    <t>A last name (or surname) is the family name passed down from one generation to the next for the individual conducting the study.</t>
   </si>
   <si>
     <t>e.g. Doe</t>
   </si>
   <si>
-    <t>An organization that this person is affiliated with. For example, a school/university, a club, or a team.</t>
+    <t>A unique identifier used to send and receive electronic messages (emails) over the internet.</t>
+  </si>
+  <si>
+    <t>e.g. jane.doe@example.com</t>
+  </si>
+  <si>
+    <t>An organisation or institution that this person is associated with.</t>
   </si>
   <si>
     <t>e.g. University of Liverpool</t>
@@ -197,7 +221,7 @@
     <t>e.g. BBSRC</t>
   </si>
   <si>
-    <t>A Grant that directly or indirectly provide funding or sponsorship for this item.</t>
+    <t>A grant that directly or indirectly provides funding or sponsorship for the person to conduct the study.</t>
   </si>
   <si>
     <t>e.g. GRAK3489</t>
@@ -758,7 +782,7 @@
     <t>The date on which the subject was determined as representing the dwc:Taxon.</t>
   </si>
   <si>
-    <t>e.g. 1963-03-08T14: 07-0600</t>
+    <t>e.g. 1963-03-08T14:07</t>
   </si>
   <si>
     <t>The current state of a specimen with respect to the collection identified in dwc:collectionCode or dwc:collectionID.</t>
@@ -1928,10 +1952,350 @@
     <t>e.g. 75</t>
   </si>
   <si>
+    <t>file_derived_from</t>
+  </si>
+  <si>
+    <t>inferred_cell_type</t>
+  </si>
+  <si>
+    <t>post_analysis_cell_well_quality</t>
+  </si>
+  <si>
+    <t>other_derived_cell_attributes</t>
+  </si>
+  <si>
+    <t>file_derived_from (optional)</t>
+  </si>
+  <si>
+    <t>inferred_cell_type (optional)</t>
+  </si>
+  <si>
+    <t>post_analysis_cell_well_quality (optional)</t>
+  </si>
+  <si>
+    <t>other_derived_cell_attributes (optional)</t>
+  </si>
+  <si>
+    <t>The name of the file that was used to generate the analysis derived data.</t>
+  </si>
+  <si>
+    <t>e.g. file1_sequencing.json</t>
+  </si>
+  <si>
+    <t>Post analysis cell type or identity declaration based on expression profile or known gene function identified by the performer.</t>
+  </si>
+  <si>
+    <t>e.g. type II bipolar neuron</t>
+  </si>
+  <si>
+    <t>Performer defined measure of whether the read output
+from the cell was included in the sequencing analysis. For example, cells might be excluded if a threshold percentage of reads did not map to the genome or if pre-sequencing quality measures were not passed.</t>
+  </si>
+  <si>
+    <t>e.g. Passed</t>
+  </si>
+  <si>
+    <t>Any other cell level measurement or annotation as result of the analysis.</t>
+  </si>
+  <si>
+    <t>e.g. cluster</t>
+  </si>
+  <si>
+    <t>reference_genome</t>
+  </si>
+  <si>
+    <t>genome_annotation</t>
+  </si>
+  <si>
+    <t>annotation_filtering</t>
+  </si>
+  <si>
+    <t>genes_vs_exons</t>
+  </si>
+  <si>
+    <t>library_structure</t>
+  </si>
+  <si>
+    <t>mapping_and_demultiplexing_software</t>
+  </si>
+  <si>
+    <t>read_mapping_statistics</t>
+  </si>
+  <si>
+    <t>sequencing_saturation</t>
+  </si>
+  <si>
+    <t>umis_barcode_distribution_qc</t>
+  </si>
+  <si>
+    <t>cell_non_cell_filtering_strategy</t>
+  </si>
+  <si>
+    <t>other_quality_filters_applied</t>
+  </si>
+  <si>
+    <t>ambient_rna_qc</t>
+  </si>
+  <si>
+    <t>predicted_doublet_rate_qc</t>
+  </si>
+  <si>
+    <t>individual_organism_snp_demultiplexing</t>
+  </si>
+  <si>
+    <t>reference_genome (optional)</t>
+  </si>
+  <si>
+    <t>genome_annotation (optional)</t>
+  </si>
+  <si>
+    <t>annotation_filtering (optional)</t>
+  </si>
+  <si>
+    <t>genes_vs_exons (optional)</t>
+  </si>
+  <si>
+    <t>library_structure (optional)</t>
+  </si>
+  <si>
+    <t>mapping_and_demultiplexing_software (optional)</t>
+  </si>
+  <si>
+    <t>read_mapping_statistics (optional)</t>
+  </si>
+  <si>
+    <t>sequencing_saturation (optional)</t>
+  </si>
+  <si>
+    <t>umis_barcode_distribution_qc (optional)</t>
+  </si>
+  <si>
+    <t>cell_non_cell_filtering_strategy (optional)</t>
+  </si>
+  <si>
+    <t>other_quality_filters_applied (optional)</t>
+  </si>
+  <si>
+    <t>ambient_rna_qc (optional)</t>
+  </si>
+  <si>
+    <t>predicted_doublet_rate_qc (optional)</t>
+  </si>
+  <si>
+    <t>individual_organism_snp_demultiplexing (optional)</t>
+  </si>
+  <si>
+    <t>Indicate version and include stable link to genome data (or attach genome fasta file).</t>
+  </si>
+  <si>
+    <t>e.g. GRCh38, https://example.org/grch38.fa</t>
+  </si>
+  <si>
+    <t>Indicate version and include stable link. Also indicate if any modification to the original annotation has been applied (e.g. 3' UTR extension) and include modified annotation file employed in the analysis.</t>
+  </si>
+  <si>
+    <t>e.g. Ensembl v101, https://example.org/ensembl_v101.gtf</t>
+  </si>
+  <si>
+    <t>Indicate which features were filtered (i.e. protein coding, pseudo-genes, TCRs, etc.)</t>
+  </si>
+  <si>
+    <t>e.g. Filtered to include only protein-coding genes</t>
+  </si>
+  <si>
+    <t>Quantification using whole gene intervals or exons.</t>
+  </si>
+  <si>
+    <t>e.g. Exon quantification</t>
+  </si>
+  <si>
+    <t>seqspec format</t>
+  </si>
+  <si>
+    <t>e.g. Single-cell 3' library</t>
+  </si>
+  <si>
+    <t>Reads/UMI</t>
+  </si>
+  <si>
+    <t>e.g. Cell Ranger 6.0.0</t>
+  </si>
+  <si>
+    <t>Statistics of the Reads or Unique Molecular Identifier (UMI).</t>
+  </si>
+  <si>
+    <t>e.g. 80% reads mapped to reference</t>
+  </si>
+  <si>
+    <t>Depending on number of cells recovered (not targeted) and technology</t>
+  </si>
+  <si>
+    <t>e.g. 95% sequencing saturation</t>
+  </si>
+  <si>
+    <t>Show Unique Molecular Identifiers (UMIs) per barcode distribution and threshold applied</t>
+  </si>
+  <si>
+    <t>e.g. Threshold: 10 UMIs per barcode</t>
+  </si>
+  <si>
+    <t>Unique Molecular Identifier (UMI) threshold used to discriminate cells from non-cells. Description of algorithm (if any) and parameters used to determine cells or non-cells.</t>
+  </si>
+  <si>
+    <t>e.g. Threshold: 5 UMIs for cell detection</t>
+  </si>
+  <si>
+    <t>Cells/nuclei discarded based on % mitochondrial reads, % rRNA reads, etc.</t>
+  </si>
+  <si>
+    <t>e.g. Cells with &gt;20% mitochondrial reads discarded</t>
+  </si>
+  <si>
+    <t>Report % UMIs in background cell barcodes, and algorithm (if any) used to remove ambient RNA</t>
+  </si>
+  <si>
+    <t>e.g. Ambient RNA removed if &gt;5% UMIs in background barcodes</t>
+  </si>
+  <si>
+    <t>e.g. Predicted doublet rate: 1.5%</t>
+  </si>
+  <si>
+    <t>If carried out, show SNP partitioning quality (e.g. SNP UMAP embedding or covariance matrix), algorithm used</t>
+  </si>
+  <si>
+    <t>e.g. SNP UMAP embedding using CellSNP</t>
+  </si>
+  <si>
+    <t>clustering_algorithm_and_version</t>
+  </si>
+  <si>
+    <t>clustering_parameters</t>
+  </si>
+  <si>
+    <t>integration_batch_correction</t>
+  </si>
+  <si>
+    <t>clustering_algorithm_and_version (optional)</t>
+  </si>
+  <si>
+    <t>clustering_parameters (optional)</t>
+  </si>
+  <si>
+    <t>integration_batch_correction (optional)</t>
+  </si>
+  <si>
+    <t>If compared/integrated with existing datasets</t>
+  </si>
+  <si>
+    <t>e.g. Louvain 0.8.0</t>
+  </si>
+  <si>
+    <t>e.g. Resolution: 0.6, K-nearest neighbors: 10</t>
+  </si>
+  <si>
+    <t>e.g. Harmony v1.0</t>
+  </si>
+  <si>
+    <t>source_code</t>
+  </si>
+  <si>
+    <t>umi_count_matrix</t>
+  </si>
+  <si>
+    <t>ensembl_ids</t>
+  </si>
+  <si>
+    <t>functional_gene_annotations</t>
+  </si>
+  <si>
+    <t>protein_models</t>
+  </si>
+  <si>
+    <t>cell_metadata</t>
+  </si>
+  <si>
+    <t>cluster_level_normalised_expression_tables</t>
+  </si>
+  <si>
+    <t>other_resource_files</t>
+  </si>
+  <si>
+    <t>source_code (optional)</t>
+  </si>
+  <si>
+    <t>umi_count_matrix (optional)</t>
+  </si>
+  <si>
+    <t>ensembl_ids (optional)</t>
+  </si>
+  <si>
+    <t>functional_gene_annotations (optional)</t>
+  </si>
+  <si>
+    <t>protein_models (optional)</t>
+  </si>
+  <si>
+    <t>cell_metadata (optional)</t>
+  </si>
+  <si>
+    <t>cluster_level_normalised_expression_tables (optional)</t>
+  </si>
+  <si>
+    <t>other_resource_files (optional)</t>
+  </si>
+  <si>
+    <t>If any newly developed code/software has been used in the processing and downstream analysis of the dataset.</t>
+  </si>
+  <si>
+    <t>e.g. Source code is hosted on GitHub and includes custom algorithms for UMI count normalization. The repository can be found at: https://github.com/user/umi-normalization.</t>
+  </si>
+  <si>
+    <t>Gene x cell matrix with UMI counts for each gene in each cell.</t>
+  </si>
+  <si>
+    <t>e.g. The UMI count matrix is stored in a CSV file with gene IDs as rows (e.g., ENSG00000139618) and cell barcodes as columns (e.g., Cell_001, Cell_002). The matrix file is available at: https://example.com/umi_count_matrix.csv.</t>
+  </si>
+  <si>
+    <t>Gene or transcript names should be listed as Ensembl (or other standardized ID), with gene short names in metadata.</t>
+  </si>
+  <si>
+    <t>e.g. ENSG00000139618</t>
+  </si>
+  <si>
+    <t>Any functional annotation generated/used (gene names, GOs, structural domains, etc.).</t>
+  </si>
+  <si>
+    <t>e.g. Functional gene annotations, including Gene Ontology (GO) terms, are provided in the metadata. For example, the gene 'ENSG00000139618' (BRCA1) is annotated with the GO term 'GO:0003674' (DNA binding).</t>
+  </si>
+  <si>
+    <t>FASTA file with (or stable link to) the predicted proteins associated to genes in the UMI count matrix and matching IDs.</t>
+  </si>
+  <si>
+    <t>e.g. The protein sequences for genes are provided in a FASTA file available at: https://example.com/protein_models.fasta, where each protein sequence is linked to the corresponding gene ID.</t>
+  </si>
+  <si>
+    <t>Table mapping cell IDs to cluster/cell type/broad cell type annotations.</t>
+  </si>
+  <si>
+    <t>e.g. Cell metadata includes information such as cell type annotations ('Tumor', 'Normal') and experimental conditions ('Control', 'Treatment'). This data is available in a table at: https://example.com/cell_metadata.csv.</t>
+  </si>
+  <si>
+    <t>Expression tables that show normalised gene expression at the cluster or cell-type level.</t>
+  </si>
+  <si>
+    <t>e.g. Normalised gene expression data at the cluster level is provided in a tab-delimited text file. For example, gene 'ENSG00000139618' (BRCA1) has expression values for clusters: Cluster_1: 1200, Cluster_2: 900. The full expression table is available at: https://example.com/cluster_level_expression.csv.</t>
+  </si>
+  <si>
+    <t>Necessary to re-use and interpret the data. E.g. barcode information in complex, serial multiplexing protocols (clicktags).</t>
+  </si>
+  <si>
+    <t>e.g. Barcode information used in multiplexing protocols is provided in a separate file, which can be accessed at: https://example.com/barcode_data.csv.</t>
+  </si>
+  <si>
+    <t>lib_prep_id</t>
+  </si>
+  <si>
     <t>file_id</t>
-  </si>
-  <si>
-    <t>lib_prep_id</t>
   </si>
   <si>
     <t>read_1_file</t>
@@ -2022,7 +2386,7 @@
     <t>e.g. file001</t>
   </si>
   <si>
-    <t>A file type is a name given to a specific kind of file. Common file types are fastq, gtf, fasta, bam, etc.</t>
+    <t>A file type is a name given to a specific kind of file. Common file types are fastq, gtf, fasta, bam, archive etc.</t>
   </si>
   <si>
     <t>e.g. fastq</t>
@@ -2032,346 +2396,6 @@
   </si>
   <si>
     <t>e.g. filename1.txt</t>
-  </si>
-  <si>
-    <t>file_derived_from</t>
-  </si>
-  <si>
-    <t>inferred_cell_type</t>
-  </si>
-  <si>
-    <t>post_analysis_cell_well_quality</t>
-  </si>
-  <si>
-    <t>other_derived_cell_attributes</t>
-  </si>
-  <si>
-    <t>file_derived_from (optional)</t>
-  </si>
-  <si>
-    <t>inferred_cell_type (optional)</t>
-  </si>
-  <si>
-    <t>post_analysis_cell_well_quality (optional)</t>
-  </si>
-  <si>
-    <t>other_derived_cell_attributes (optional)</t>
-  </si>
-  <si>
-    <t>The name of the file that was used to generate the analysis derived data.</t>
-  </si>
-  <si>
-    <t>e.g. file1_sequencing.json</t>
-  </si>
-  <si>
-    <t>Post analysis cell type or identity declaration based on expression profile or known gene function identified by the performer.</t>
-  </si>
-  <si>
-    <t>e.g. type II bipolar neuron</t>
-  </si>
-  <si>
-    <t>Performer defined measure of whether the read output
-from the cell was included in the sequencing analysis. For example, cells might be excluded if a threshold percentage of reads did not map to the genome or if pre-sequencing quality measures were not passed.</t>
-  </si>
-  <si>
-    <t>e.g. Passed</t>
-  </si>
-  <si>
-    <t>Any other cell level measurement or annotation as result of the analysis.</t>
-  </si>
-  <si>
-    <t>e.g. cluster</t>
-  </si>
-  <si>
-    <t>reference_genome</t>
-  </si>
-  <si>
-    <t>genome_annotation</t>
-  </si>
-  <si>
-    <t>annotation_filtering</t>
-  </si>
-  <si>
-    <t>genes_vs_exons</t>
-  </si>
-  <si>
-    <t>library_structure</t>
-  </si>
-  <si>
-    <t>mapping_and_demultiplexing_software</t>
-  </si>
-  <si>
-    <t>read_mapping_statistics</t>
-  </si>
-  <si>
-    <t>sequencing_saturation</t>
-  </si>
-  <si>
-    <t>umis_barcode_distribution_qc</t>
-  </si>
-  <si>
-    <t>cell_non_cell_filtering_strategy</t>
-  </si>
-  <si>
-    <t>other_quality_filters_applied</t>
-  </si>
-  <si>
-    <t>ambient_rna_qc</t>
-  </si>
-  <si>
-    <t>predicted_doublet_rate_qc</t>
-  </si>
-  <si>
-    <t>individual_organism_snp_demultiplexing</t>
-  </si>
-  <si>
-    <t>reference_genome (optional)</t>
-  </si>
-  <si>
-    <t>genome_annotation (optional)</t>
-  </si>
-  <si>
-    <t>annotation_filtering (optional)</t>
-  </si>
-  <si>
-    <t>genes_vs_exons (optional)</t>
-  </si>
-  <si>
-    <t>library_structure (optional)</t>
-  </si>
-  <si>
-    <t>mapping_and_demultiplexing_software (optional)</t>
-  </si>
-  <si>
-    <t>read_mapping_statistics (optional)</t>
-  </si>
-  <si>
-    <t>sequencing_saturation (optional)</t>
-  </si>
-  <si>
-    <t>umis_barcode_distribution_qc (optional)</t>
-  </si>
-  <si>
-    <t>cell_non_cell_filtering_strategy (optional)</t>
-  </si>
-  <si>
-    <t>other_quality_filters_applied (optional)</t>
-  </si>
-  <si>
-    <t>ambient_rna_qc (optional)</t>
-  </si>
-  <si>
-    <t>predicted_doublet_rate_qc (optional)</t>
-  </si>
-  <si>
-    <t>individual_organism_snp_demultiplexing (optional)</t>
-  </si>
-  <si>
-    <t>Indicate version and include stable link to genome data (or attach genome fasta file).</t>
-  </si>
-  <si>
-    <t>e.g. GRCh38, https://example.org/grch38.fa</t>
-  </si>
-  <si>
-    <t>Indicate version and include stable link. Also indicate if any modification to the original annotation has been applied (e.g. 3' UTR extension) and include modified annotation file employed in the analysis.</t>
-  </si>
-  <si>
-    <t>e.g. Ensembl v101, https://example.org/ensembl_v101.gtf</t>
-  </si>
-  <si>
-    <t>Indicate which features were filtered (i.e. protein coding, pseudo-genes, TCRs, etc.)</t>
-  </si>
-  <si>
-    <t>e.g. Filtered to include only protein-coding genes</t>
-  </si>
-  <si>
-    <t>Quantification using whole gene intervals or exons.</t>
-  </si>
-  <si>
-    <t>e.g. Exon quantification</t>
-  </si>
-  <si>
-    <t>seqspec format</t>
-  </si>
-  <si>
-    <t>e.g. Single-cell 3' library</t>
-  </si>
-  <si>
-    <t>Reads/UMI</t>
-  </si>
-  <si>
-    <t>e.g. Cell Ranger 6.0.0</t>
-  </si>
-  <si>
-    <t>Statistics of the Reads or Unique Molecular Identifier (UMI).</t>
-  </si>
-  <si>
-    <t>e.g. 80% reads mapped to reference</t>
-  </si>
-  <si>
-    <t>Depending on number of cells recovered (not targeted) and technology</t>
-  </si>
-  <si>
-    <t>e.g. 95% sequencing saturation</t>
-  </si>
-  <si>
-    <t>Show Unique Molecular Identifiers (UMIs) per barcode distribution and threshold applied</t>
-  </si>
-  <si>
-    <t>e.g. Threshold: 10 UMIs per barcode</t>
-  </si>
-  <si>
-    <t>Unique Molecular Identifier (UMI) threshold used to discriminate cells from non-cells. Description of algorithm (if any) and parameters used to determine cells or non-cells.</t>
-  </si>
-  <si>
-    <t>e.g. Threshold: 5 UMIs for cell detection</t>
-  </si>
-  <si>
-    <t>Cells/nuclei discarded based on % mitochondrial reads, % rRNA reads, etc.</t>
-  </si>
-  <si>
-    <t>e.g. Cells with &gt;20% mitochondrial reads discarded</t>
-  </si>
-  <si>
-    <t>Report % UMIs in background cell barcodes, and algorithm (if any) used to remove ambient RNA</t>
-  </si>
-  <si>
-    <t>e.g. Ambient RNA removed if &gt;5% UMIs in background barcodes</t>
-  </si>
-  <si>
-    <t>e.g. Predicted doublet rate: 1.5%</t>
-  </si>
-  <si>
-    <t>If carried out, show SNP partitioning quality (e.g. SNP UMAP embedding or covariance matrix), algorithm used</t>
-  </si>
-  <si>
-    <t>e.g. SNP UMAP embedding using CellSNP</t>
-  </si>
-  <si>
-    <t>clustering_algorithm_and_version</t>
-  </si>
-  <si>
-    <t>clustering_parameters</t>
-  </si>
-  <si>
-    <t>integration_batch_correction</t>
-  </si>
-  <si>
-    <t>clustering_algorithm_and_version (optional)</t>
-  </si>
-  <si>
-    <t>clustering_parameters (optional)</t>
-  </si>
-  <si>
-    <t>integration_batch_correction (optional)</t>
-  </si>
-  <si>
-    <t>If compared/integrated with existing datasets</t>
-  </si>
-  <si>
-    <t>e.g. Louvain 0.8.0</t>
-  </si>
-  <si>
-    <t>e.g. Resolution: 0.6, K-nearest neighbors: 10</t>
-  </si>
-  <si>
-    <t>e.g. Harmony v1.0</t>
-  </si>
-  <si>
-    <t>source_code</t>
-  </si>
-  <si>
-    <t>umi_count_matrix</t>
-  </si>
-  <si>
-    <t>ensembl_ids</t>
-  </si>
-  <si>
-    <t>functional_gene_annotations</t>
-  </si>
-  <si>
-    <t>protein_models</t>
-  </si>
-  <si>
-    <t>cell_metadata</t>
-  </si>
-  <si>
-    <t>cluster_level_normalised_expression_tables</t>
-  </si>
-  <si>
-    <t>other_resource_files</t>
-  </si>
-  <si>
-    <t>source_code (optional)</t>
-  </si>
-  <si>
-    <t>umi_count_matrix (optional)</t>
-  </si>
-  <si>
-    <t>ensembl_ids (optional)</t>
-  </si>
-  <si>
-    <t>functional_gene_annotations (optional)</t>
-  </si>
-  <si>
-    <t>protein_models (optional)</t>
-  </si>
-  <si>
-    <t>cell_metadata (optional)</t>
-  </si>
-  <si>
-    <t>cluster_level_normalised_expression_tables (optional)</t>
-  </si>
-  <si>
-    <t>other_resource_files (optional)</t>
-  </si>
-  <si>
-    <t>If any newly developed code/software has been used in the processing and downstream analysis of the dataset.</t>
-  </si>
-  <si>
-    <t>e.g. Source code is hosted on GitHub and includes custom algorithms for UMI count normalization. The repository can be found at: https://github.com/user/umi-normalization.</t>
-  </si>
-  <si>
-    <t>Gene x cell matrix with UMI counts for each gene in each cell.</t>
-  </si>
-  <si>
-    <t>e.g. The UMI count matrix is stored in a CSV file with gene IDs as rows (e.g., ENSG00000139618) and cell barcodes as columns (e.g., Cell_001, Cell_002). The matrix file is available at: https://example.com/umi_count_matrix.csv.</t>
-  </si>
-  <si>
-    <t>Gene or transcript names should be listed as Ensembl (or other standardized ID), with gene short names in metadata.</t>
-  </si>
-  <si>
-    <t>e.g. The UMI count matrix includes genes identified by their Ensembl IDs, such as 'ENSG00000139618' for the BRCA1 gene. See the full list of Ensembl IDs in the metadata file.</t>
-  </si>
-  <si>
-    <t>Any functional annotation generated/used (gene names, GOs, structural domains, etc.).</t>
-  </si>
-  <si>
-    <t>e.g. Functional gene annotations, including Gene Ontology (GO) terms, are provided in the metadata. For example, the gene 'ENSG00000139618' (BRCA1) is annotated with the GO term 'GO:0003674' (DNA binding).</t>
-  </si>
-  <si>
-    <t>FASTA file with (or stable link to) the predicted proteins associated to genes in the UMI count matrix and matching IDs.</t>
-  </si>
-  <si>
-    <t>e.g. The protein sequences for genes are provided in a FASTA file available at: https://example.com/protein_models.fasta, where each protein sequence is linked to the corresponding gene ID.</t>
-  </si>
-  <si>
-    <t>Table mapping cell IDs to cluster/cell type/broad cell type annotations.</t>
-  </si>
-  <si>
-    <t>e.g. Cell metadata includes information such as cell type annotations ('Tumor', 'Normal') and experimental conditions ('Control', 'Treatment'). This data is available in a table at: https://example.com/cell_metadata.csv.</t>
-  </si>
-  <si>
-    <t>Expression tables that show normalised gene expression at the cluster or cell-type level.</t>
-  </si>
-  <si>
-    <t>e.g. Normalised gene expression data at the cluster level is provided in a tab-delimited text file. For example, gene 'ENSG00000139618' (BRCA1) has expression values for clusters: Cluster_1: 1200, Cluster_2: 900. The full expression table is available at: https://example.com/cluster_level_expression.csv.</t>
-  </si>
-  <si>
-    <t>Necessary to re-use and interpret the data. E.g. barcode information in complex, serial multiplexing protocols (clicktags).</t>
-  </si>
-  <si>
-    <t>e.g. Barcode information used in multiplexing protocols is provided in a separate file, which can be accessed at: https://example.com/barcode_data.csv.</t>
   </si>
 </sst>
 </file>
@@ -2763,8 +2787,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="197.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -2811,198 +2835,12 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="A343" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="88DF" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="42.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="98.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="48.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="49.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="193.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="195.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="80.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="88.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="126.42578125" style="4" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>633</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>590</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>635</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>636</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>637</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>638</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>639</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>640</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>645</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>642</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>643</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>647</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>542</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>648</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>650</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>654</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>656</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>658</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>660</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>662</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>664</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>543</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>612</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>649</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>651</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>653</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>657</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>659</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>661</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>663</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>665</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-    </row>
-  </sheetData>
-  <sheetProtection password="EA39" sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="1">
-    <mergeCell ref="A4:N4"/>
-  </mergeCells>
-  <conditionalFormatting sqref="A1:N4">
-    <cfRule type="notContainsErrors" dxfId="0" priority="1">
-      <formula>NOT(ISERROR(A1))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -3022,16 +2860,16 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>672</v>
+        <v>645</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>673</v>
+        <v>646</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>674</v>
+        <v>647</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>675</v>
+        <v>648</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3039,16 +2877,16 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>676</v>
+        <v>649</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>678</v>
+        <v>651</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>680</v>
+        <v>653</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>682</v>
+        <v>655</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3056,16 +2894,16 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>677</v>
+        <v>650</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>679</v>
+        <v>652</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>681</v>
+        <v>654</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>683</v>
+        <v>656</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3078,7 +2916,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A0D8" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="AA49" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -3099,7 +2937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O4"/>
   <sheetViews>
@@ -3129,46 +2967,46 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>698</v>
+        <v>671</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>699</v>
+        <v>672</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>700</v>
+        <v>673</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>701</v>
+        <v>674</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>702</v>
+        <v>675</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>703</v>
+        <v>676</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>704</v>
+        <v>677</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>705</v>
+        <v>678</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>706</v>
+        <v>679</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>707</v>
+        <v>680</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>708</v>
+        <v>681</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>709</v>
+        <v>682</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>710</v>
+        <v>683</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>711</v>
+        <v>684</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -3176,46 +3014,46 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>712</v>
+        <v>685</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>714</v>
+        <v>687</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>716</v>
+        <v>689</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>718</v>
+        <v>691</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>720</v>
+        <v>693</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>722</v>
+        <v>695</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>724</v>
+        <v>697</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>726</v>
+        <v>699</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>728</v>
+        <v>701</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>730</v>
+        <v>703</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>732</v>
+        <v>705</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>734</v>
+        <v>707</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>726</v>
+        <v>699</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>737</v>
+        <v>710</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -3223,46 +3061,46 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>713</v>
+        <v>686</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>715</v>
+        <v>688</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>717</v>
+        <v>690</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>719</v>
+        <v>692</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>721</v>
+        <v>694</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>723</v>
+        <v>696</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>725</v>
+        <v>698</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>727</v>
+        <v>700</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>729</v>
+        <v>702</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>731</v>
+        <v>704</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>733</v>
+        <v>706</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>735</v>
+        <v>708</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>736</v>
+        <v>709</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>738</v>
+        <v>711</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -3285,7 +3123,7 @@
       <c r="O4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="AA78" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="ADDF" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>
   </mergeCells>
@@ -3298,7 +3136,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -3315,13 +3153,13 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>742</v>
+        <v>715</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>743</v>
+        <v>716</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>744</v>
+        <v>717</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3329,13 +3167,13 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>745</v>
+        <v>718</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>745</v>
+        <v>718</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>745</v>
+        <v>718</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3343,13 +3181,13 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>746</v>
+        <v>719</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>747</v>
+        <v>720</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>748</v>
+        <v>721</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3361,7 +3199,7 @@
       <c r="D4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A998" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="95DE" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
   </mergeCells>
@@ -3374,7 +3212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -3384,7 +3222,7 @@
   <cols>
     <col min="1" max="1" width="154.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="198.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="152.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="103.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="187.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="170.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="191.7109375" style="4" bestFit="1" customWidth="1"/>
@@ -3394,80 +3232,80 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>757</v>
+        <v>730</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>758</v>
+        <v>731</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>759</v>
+        <v>732</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>760</v>
+        <v>733</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>761</v>
+        <v>734</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>762</v>
+        <v>735</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>763</v>
+        <v>736</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>764</v>
+        <v>737</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>765</v>
+        <v>738</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>767</v>
+        <v>740</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>769</v>
+        <v>742</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>771</v>
+        <v>744</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>773</v>
+        <v>746</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>775</v>
+        <v>748</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>777</v>
+        <v>750</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>779</v>
+        <v>752</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
-        <v>766</v>
+        <v>739</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>768</v>
+        <v>741</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>770</v>
+        <v>743</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>772</v>
+        <v>745</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>774</v>
+        <v>747</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>776</v>
+        <v>749</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>778</v>
+        <v>751</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>780</v>
+        <v>753</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3483,11 +3321,197 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="B016" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="CEF1" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:H4">
+    <cfRule type="notContainsErrors" dxfId="0" priority="1">
+      <formula>NOT(ISERROR(A1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="42.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="98.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="48.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="49.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="193.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="195.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="80.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="95.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="126.42578125" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>550</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>768</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>769</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>771</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>775</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>777</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>779</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>781</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>783</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>785</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>620</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>770</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>772</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>774</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>776</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>778</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>780</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>786</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+    </row>
+  </sheetData>
+  <sheetProtection password="F573" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A4:N4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A1:N4">
     <cfRule type="notContainsErrors" dxfId="0" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
@@ -3594,7 +3618,7 @@
       <c r="G4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="F2F4" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="F197" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:G4"/>
   </mergeCells>
@@ -3629,7 +3653,7 @@
   <sheetData>
     <row r="5" spans="5:6">
       <c r="E5" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="F5" t="s">
         <v>33</v>
@@ -3637,7 +3661,7 @@
     </row>
     <row r="6" spans="5:6">
       <c r="E6" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
       <c r="F6" t="s">
         <v>34</v>
@@ -3645,7 +3669,7 @@
     </row>
     <row r="7" spans="5:6">
       <c r="E7" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="F7" t="s">
         <v>35</v>
@@ -3653,7 +3677,7 @@
     </row>
     <row r="8" spans="5:6">
       <c r="E8" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="F8" t="s">
         <v>36</v>
@@ -3661,7 +3685,7 @@
     </row>
     <row r="9" spans="5:6">
       <c r="E9" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
       <c r="F9" t="s">
         <v>37</v>
@@ -3669,7 +3693,7 @@
     </row>
     <row r="10" spans="5:6">
       <c r="E10" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="F10" t="s">
         <v>38</v>
@@ -3677,7 +3701,7 @@
     </row>
     <row r="11" spans="5:6">
       <c r="E11" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
       <c r="F11" t="s">
         <v>39</v>
@@ -3685,7 +3709,7 @@
     </row>
     <row r="12" spans="5:6">
       <c r="E12" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="F12" t="s">
         <v>40</v>
@@ -3693,337 +3717,337 @@
     </row>
     <row r="13" spans="5:6">
       <c r="E13" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
     </row>
     <row r="14" spans="5:6">
       <c r="E14" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
     </row>
     <row r="15" spans="5:6">
       <c r="E15" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
     </row>
     <row r="16" spans="5:6">
       <c r="E16" t="s">
-        <v>361</v>
+        <v>369</v>
       </c>
     </row>
     <row r="17" spans="5:5">
       <c r="E17" t="s">
-        <v>362</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18" spans="5:5">
       <c r="E18" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
     </row>
     <row r="19" spans="5:5">
       <c r="E19" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
     </row>
     <row r="20" spans="5:5">
       <c r="E20" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
     </row>
     <row r="21" spans="5:5">
       <c r="E21" t="s">
-        <v>366</v>
+        <v>374</v>
       </c>
     </row>
     <row r="22" spans="5:5">
       <c r="E22" t="s">
-        <v>367</v>
+        <v>375</v>
       </c>
     </row>
     <row r="23" spans="5:5">
       <c r="E23" t="s">
-        <v>368</v>
+        <v>376</v>
       </c>
     </row>
     <row r="24" spans="5:5">
       <c r="E24" t="s">
-        <v>369</v>
+        <v>377</v>
       </c>
     </row>
     <row r="25" spans="5:5">
       <c r="E25" t="s">
-        <v>370</v>
+        <v>378</v>
       </c>
     </row>
     <row r="26" spans="5:5">
       <c r="E26" t="s">
-        <v>371</v>
+        <v>379</v>
       </c>
     </row>
     <row r="27" spans="5:5">
       <c r="E27" t="s">
-        <v>372</v>
+        <v>380</v>
       </c>
     </row>
     <row r="28" spans="5:5">
       <c r="E28" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
     </row>
     <row r="29" spans="5:5">
       <c r="E29" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
     </row>
     <row r="30" spans="5:5">
       <c r="E30" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
     </row>
     <row r="31" spans="5:5">
       <c r="E31" t="s">
-        <v>376</v>
+        <v>384</v>
       </c>
     </row>
     <row r="32" spans="5:5">
       <c r="E32" t="s">
-        <v>377</v>
+        <v>385</v>
       </c>
     </row>
     <row r="33" spans="5:5">
       <c r="E33" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
     </row>
     <row r="34" spans="5:5">
       <c r="E34" t="s">
-        <v>379</v>
+        <v>387</v>
       </c>
     </row>
     <row r="35" spans="5:5">
       <c r="E35" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
     </row>
     <row r="36" spans="5:5">
       <c r="E36" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
     </row>
     <row r="37" spans="5:5">
       <c r="E37" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="38" spans="5:5">
       <c r="E38" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
     </row>
     <row r="39" spans="5:5">
       <c r="E39" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
     </row>
     <row r="40" spans="5:5">
       <c r="E40" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
     </row>
     <row r="41" spans="5:5">
       <c r="E41" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
     </row>
     <row r="42" spans="5:5">
       <c r="E42" t="s">
-        <v>387</v>
+        <v>395</v>
       </c>
     </row>
     <row r="43" spans="5:5">
       <c r="E43" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
     </row>
     <row r="44" spans="5:5">
       <c r="E44" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
     </row>
     <row r="45" spans="5:5">
       <c r="E45" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
     </row>
     <row r="46" spans="5:5">
       <c r="E46" t="s">
-        <v>391</v>
+        <v>399</v>
       </c>
     </row>
     <row r="47" spans="5:5">
       <c r="E47" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
     </row>
     <row r="48" spans="5:5">
       <c r="E48" t="s">
-        <v>393</v>
+        <v>401</v>
       </c>
     </row>
     <row r="49" spans="5:5">
       <c r="E49" t="s">
-        <v>394</v>
+        <v>402</v>
       </c>
     </row>
     <row r="50" spans="5:5">
       <c r="E50" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
     </row>
     <row r="51" spans="5:5">
       <c r="E51" t="s">
-        <v>396</v>
+        <v>404</v>
       </c>
     </row>
     <row r="52" spans="5:5">
       <c r="E52" t="s">
-        <v>397</v>
+        <v>405</v>
       </c>
     </row>
     <row r="53" spans="5:5">
       <c r="E53" t="s">
-        <v>398</v>
+        <v>406</v>
       </c>
     </row>
     <row r="54" spans="5:5">
       <c r="E54" t="s">
-        <v>399</v>
+        <v>407</v>
       </c>
     </row>
     <row r="55" spans="5:5">
       <c r="E55" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
     </row>
     <row r="56" spans="5:5">
       <c r="E56" t="s">
-        <v>401</v>
+        <v>409</v>
       </c>
     </row>
     <row r="57" spans="5:5">
       <c r="E57" t="s">
-        <v>402</v>
+        <v>410</v>
       </c>
     </row>
     <row r="58" spans="5:5">
       <c r="E58" t="s">
-        <v>403</v>
+        <v>411</v>
       </c>
     </row>
     <row r="59" spans="5:5">
       <c r="E59" t="s">
-        <v>404</v>
+        <v>412</v>
       </c>
     </row>
     <row r="60" spans="5:5">
       <c r="E60" t="s">
-        <v>405</v>
+        <v>413</v>
       </c>
     </row>
     <row r="61" spans="5:5">
       <c r="E61" t="s">
-        <v>406</v>
+        <v>414</v>
       </c>
     </row>
     <row r="62" spans="5:5">
       <c r="E62" t="s">
-        <v>407</v>
+        <v>415</v>
       </c>
     </row>
     <row r="63" spans="5:5">
       <c r="E63" t="s">
-        <v>408</v>
+        <v>416</v>
       </c>
     </row>
     <row r="64" spans="5:5">
       <c r="E64" t="s">
-        <v>409</v>
+        <v>417</v>
       </c>
     </row>
     <row r="65" spans="5:5">
       <c r="E65" t="s">
-        <v>410</v>
+        <v>418</v>
       </c>
     </row>
     <row r="66" spans="5:5">
       <c r="E66" t="s">
-        <v>411</v>
+        <v>419</v>
       </c>
     </row>
     <row r="67" spans="5:5">
       <c r="E67" t="s">
-        <v>412</v>
+        <v>420</v>
       </c>
     </row>
     <row r="68" spans="5:5">
       <c r="E68" t="s">
-        <v>413</v>
+        <v>421</v>
       </c>
     </row>
     <row r="69" spans="5:5">
       <c r="E69" t="s">
-        <v>414</v>
+        <v>422</v>
       </c>
     </row>
     <row r="70" spans="5:5">
       <c r="E70" t="s">
-        <v>415</v>
+        <v>423</v>
       </c>
     </row>
     <row r="71" spans="5:5">
       <c r="E71" t="s">
-        <v>416</v>
+        <v>424</v>
       </c>
     </row>
     <row r="72" spans="5:5">
       <c r="E72" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
     </row>
     <row r="73" spans="5:5">
       <c r="E73" t="s">
-        <v>418</v>
+        <v>426</v>
       </c>
     </row>
     <row r="74" spans="5:5">
       <c r="E74" t="s">
-        <v>419</v>
+        <v>427</v>
       </c>
     </row>
     <row r="75" spans="5:5">
       <c r="E75" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
     </row>
     <row r="76" spans="5:5">
       <c r="E76" t="s">
-        <v>421</v>
+        <v>429</v>
       </c>
     </row>
     <row r="77" spans="5:5">
       <c r="E77" t="s">
-        <v>422</v>
+        <v>430</v>
       </c>
     </row>
     <row r="78" spans="5:5">
       <c r="E78" t="s">
-        <v>423</v>
+        <v>431</v>
       </c>
     </row>
     <row r="79" spans="5:5">
       <c r="E79" t="s">
-        <v>424</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -4033,71 +4057,101 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="89.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="93.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="69.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="83.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="115.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="82.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="93.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="90.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>49</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>58</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>59</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
         <v>32</v>
       </c>
@@ -4105,13 +4159,16 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D25B" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="EAA6" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
-    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A4:H4"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:E4">
+  <conditionalFormatting sqref="A1:H4">
     <cfRule type="notContainsErrors" dxfId="0" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
@@ -4208,453 +4265,453 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="BG1" s="1" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="BI1" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="BL1" s="1" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="BM1" s="1" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="BN1" s="1" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="BP1" s="1" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="BQ1" s="1" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="BR1" s="1" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="BS1" s="1" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="BT1" s="1" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="BU1" s="1" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="BV1" s="1" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="BW1" s="1" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:75">
       <c r="A2" s="5" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="AB2" s="5" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="AF2" s="5" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="AG2" s="5" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="AH2" s="5" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="AJ2" s="5" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="AK2" s="5" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="AN2" s="5" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="AO2" s="5" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="AP2" s="5" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="AQ2" s="5" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="AR2" s="5" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="AS2" s="5" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="AT2" s="5" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="AU2" s="5" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="AV2" s="5" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="AW2" s="5" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="AX2" s="5" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="AY2" s="5" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="AZ2" s="5" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="BA2" s="5" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="BB2" s="5" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="BC2" s="5" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="BD2" s="5" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="BE2" s="5" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="BF2" s="5" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="BG2" s="5" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="BH2" s="5" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="BI2" s="5" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="BJ2" s="5" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="BK2" s="5" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="BL2" s="5" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="BM2" s="5" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="BN2" s="5" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="BO2" s="5" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="BP2" s="5" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="BQ2" s="5" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="BR2" s="5" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="BS2" s="5" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="BT2" s="5" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="BU2" s="5" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="BV2" s="5" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="BW2" s="5" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:75">
@@ -4662,226 +4719,226 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="AA3" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE3" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="AK3" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="AL3" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="AM3" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="AN3" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="AO3" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP3" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="AQ3" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="AR3" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="AS3" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="AT3" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="AU3" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="AV3" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="AW3" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="AX3" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="AY3" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="AZ3" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="AB3" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="AC3" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="AD3" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="AE3" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="AF3" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="AG3" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="AH3" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="AI3" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="AJ3" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="AK3" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="AL3" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="AM3" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="AN3" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="AO3" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="AP3" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="AQ3" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="AR3" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="AS3" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="AT3" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="AU3" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="AV3" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="AW3" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="AX3" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="AY3" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="AZ3" s="5" t="s">
-        <v>247</v>
-      </c>
       <c r="BA3" s="5" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="BB3" s="5" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="BC3" s="5" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="BD3" s="5" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="BE3" s="5" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="BF3" s="5" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="BG3" s="5" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="BH3" s="5" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="BI3" s="5" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="BJ3" s="5" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="BK3" s="5" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="BL3" s="5" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="BM3" s="5" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="BN3" s="5" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="BO3" s="5" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="BP3" s="5" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="BQ3" s="5" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="BR3" s="5" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="BS3" s="5" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="BT3" s="5" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="BU3" s="5" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="BV3" s="5" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
       <c r="BW3" s="5" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" spans="1:75">
@@ -4964,7 +5021,7 @@
       <c r="BW4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E943" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E3AE" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:BW4"/>
   </mergeCells>
@@ -5017,34 +5074,34 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>425</v>
+        <v>433</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>426</v>
+        <v>434</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>427</v>
+        <v>435</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>437</v>
+        <v>445</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>438</v>
+        <v>446</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>441</v>
+        <v>449</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -5052,34 +5109,34 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>444</v>
+        <v>452</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>450</v>
+        <v>458</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>452</v>
+        <v>460</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>454</v>
+        <v>462</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>460</v>
+        <v>468</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -5087,34 +5144,34 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>445</v>
+        <v>453</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>453</v>
+        <v>461</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>457</v>
+        <v>465</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -5133,7 +5190,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="9280" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E17B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -5180,43 +5237,43 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>425</v>
+        <v>433</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>463</v>
+        <v>471</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>474</v>
+        <v>482</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>475</v>
+        <v>483</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>476</v>
+        <v>484</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>477</v>
+        <v>485</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>478</v>
+        <v>486</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>479</v>
+        <v>487</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>480</v>
+        <v>488</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -5224,43 +5281,43 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>486</v>
+        <v>494</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>490</v>
+        <v>498</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>492</v>
+        <v>500</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>494</v>
+        <v>502</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>496</v>
+        <v>504</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>499</v>
+        <v>507</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>501</v>
+        <v>509</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>502</v>
+        <v>510</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -5268,43 +5325,43 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>483</v>
+        <v>491</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>487</v>
+        <v>495</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>493</v>
+        <v>501</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>498</v>
+        <v>506</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>500</v>
+        <v>508</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>503</v>
+        <v>511</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -5326,7 +5383,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D19E" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="D94E" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -5385,79 +5442,79 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>504</v>
+        <v>512</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>505</v>
+        <v>513</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>523</v>
-      </c>
       <c r="W1" s="1" t="s">
-        <v>538</v>
+        <v>546</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>539</v>
+        <v>547</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>541</v>
+        <v>549</v>
       </c>
     </row>
     <row r="2" spans="1:26">
@@ -5465,79 +5522,79 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>542</v>
+        <v>550</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>544</v>
+        <v>552</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>545</v>
+        <v>553</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>547</v>
+        <v>555</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>549</v>
+        <v>557</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>551</v>
+        <v>559</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>553</v>
+        <v>561</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>555</v>
+        <v>563</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>557</v>
+        <v>565</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>559</v>
+        <v>567</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>561</v>
+        <v>569</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>563</v>
+        <v>571</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>565</v>
+        <v>573</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>567</v>
+        <v>575</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>569</v>
+        <v>577</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>571</v>
+        <v>579</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>573</v>
+        <v>581</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>575</v>
+        <v>583</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>577</v>
+        <v>585</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>579</v>
+        <v>587</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>581</v>
+        <v>589</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>583</v>
+        <v>591</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>587</v>
+        <v>595</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>588</v>
+        <v>596</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -5545,79 +5602,79 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>543</v>
+        <v>551</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>546</v>
+        <v>554</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>548</v>
+        <v>556</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>550</v>
+        <v>558</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>552</v>
+        <v>560</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>554</v>
+        <v>562</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>558</v>
+        <v>566</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>560</v>
+        <v>568</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>562</v>
+        <v>570</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>564</v>
+        <v>572</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>566</v>
+        <v>574</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>568</v>
+        <v>576</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>570</v>
+        <v>578</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>572</v>
+        <v>580</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>574</v>
+        <v>582</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>576</v>
+        <v>584</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>578</v>
+        <v>586</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>580</v>
+        <v>588</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>582</v>
+        <v>590</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>586</v>
+        <v>594</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>589</v>
+        <v>597</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -5651,7 +5708,7 @@
       <c r="Z4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D705" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9794" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:Z4"/>
   </mergeCells>
@@ -5715,43 +5772,43 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>590</v>
+        <v>598</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>591</v>
+        <v>599</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>592</v>
+        <v>600</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>593</v>
+        <v>601</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>604</v>
+        <v>612</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>605</v>
+        <v>613</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>606</v>
+        <v>614</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>607</v>
+        <v>615</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>600</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>609</v>
+        <v>617</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>610</v>
+        <v>618</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -5759,43 +5816,43 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>611</v>
+        <v>619</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>613</v>
+        <v>621</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>615</v>
+        <v>623</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>617</v>
+        <v>625</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>619</v>
+        <v>627</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>621</v>
+        <v>629</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>623</v>
+        <v>631</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>624</v>
+        <v>632</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>626</v>
+        <v>634</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>626</v>
+        <v>634</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>627</v>
+        <v>635</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>629</v>
+        <v>637</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>631</v>
+        <v>639</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -5803,43 +5860,43 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>616</v>
+        <v>624</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>618</v>
+        <v>626</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>620</v>
+        <v>628</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>622</v>
+        <v>630</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>625</v>
+        <v>633</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>622</v>
+        <v>630</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>628</v>
+        <v>636</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>630</v>
+        <v>638</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>632</v>
+        <v>640</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -5861,7 +5918,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A351" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="DCCC" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Moved templates folder to 'dist' directory
</commit_message>
<xml_diff>
--- a/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.1.xlsx
+++ b/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.1.xlsx
@@ -2835,7 +2835,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="88DF" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="C3E5" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2916,7 +2916,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="AA49" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9148" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -3123,7 +3123,7 @@
       <c r="O4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="ADDF" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E90C" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>
   </mergeCells>
@@ -3199,7 +3199,7 @@
       <c r="D4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="95DE" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="CA16" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
   </mergeCells>
@@ -3321,7 +3321,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="CEF1" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E6E7" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -3507,7 +3507,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="F573" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9F83" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -3618,7 +3618,7 @@
       <c r="G4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="F197" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="CF49" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:G4"/>
   </mergeCells>
@@ -4164,7 +4164,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="EAA6" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="D8A8" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -5021,7 +5021,7 @@
       <c r="BW4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E3AE" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="F613" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:BW4"/>
   </mergeCells>
@@ -5190,7 +5190,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E17B" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="F652" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -5383,7 +5383,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D94E" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E661" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -5708,7 +5708,7 @@
       <c r="Z4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="9794" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="B3A3" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:Z4"/>
   </mergeCells>
@@ -5918,7 +5918,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="DCCC" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="BF5E" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Filled in example manifests
</commit_message>
<xml_diff>
--- a/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.1.xlsx
+++ b/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="788">
   <si>
     <t>key</t>
   </si>
@@ -53,7 +53,7 @@
     <t>Single-cell Ribonucleic Acid Sequencing (scRNA-Seq) [Darwin Core (DwC)]</t>
   </si>
   <si>
-    <t>A genomic approach for detecting and quantitatively analysing messenger Ribonucleic Acid (RNA) in individual cells, aimed at transmitting biodiversity-related information in alignment with the Darwin Core (DwC) standard.</t>
+    <t>For single cell RNA-seq studies aimed focused on biodiversity-related information in alignment with the Darwin Core (DwC) standard.</t>
   </si>
   <si>
     <t>dwc</t>
@@ -233,9 +233,6 @@
     <t>scientificName</t>
   </si>
   <si>
-    <t>organism</t>
-  </si>
-  <si>
     <t>tissue</t>
   </si>
   <si>
@@ -452,9 +449,6 @@
     <t>scientificName (optional)</t>
   </si>
   <si>
-    <t>organism (optional)</t>
-  </si>
-  <si>
     <t>tissue (optional)</t>
   </si>
   <si>
@@ -1182,6 +1176,9 @@
   </si>
   <si>
     <t>Holdfast Fungi</t>
+  </si>
+  <si>
+    <t>Inflorescence</t>
   </si>
   <si>
     <t>Intestine</t>
@@ -2788,7 +2785,7 @@
   <cols>
     <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="197.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="118.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -2835,7 +2832,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="99E8" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="F054" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2860,16 +2857,16 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>647</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2877,16 +2874,16 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2894,16 +2891,16 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2916,7 +2913,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="DCB6" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="B0C9" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -2967,46 +2964,46 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>671</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>673</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>674</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>676</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>677</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>679</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>680</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>681</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>682</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>683</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -3014,46 +3011,46 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -3061,46 +3058,46 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="M3" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>708</v>
       </c>
-      <c r="N3" s="5" t="s">
-        <v>709</v>
-      </c>
       <c r="O3" s="5" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -3123,7 +3120,7 @@
       <c r="O4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D780" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="CD84" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>
   </mergeCells>
@@ -3153,13 +3150,13 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>715</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>716</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>717</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3167,13 +3164,13 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3181,13 +3178,13 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>719</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>720</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3199,7 +3196,7 @@
       <c r="D4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="BB48" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="AFE2" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
   </mergeCells>
@@ -3232,80 +3229,80 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>730</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>733</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>735</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>736</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3321,7 +3318,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="F005" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E6F0" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -3361,43 +3358,43 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>754</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>598</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>756</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>757</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>758</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>759</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>760</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>761</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>766</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>764</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -3405,43 +3402,43 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>768</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>769</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3449,43 +3446,43 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -3507,7 +3504,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="8685" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="8224" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -3618,7 +3615,7 @@
       <c r="G4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="CE0A" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9288" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:G4"/>
   </mergeCells>
@@ -3641,413 +3638,418 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="E5:F79"/>
+  <dimension ref="D5:F80"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:6">
-      <c r="E5" t="s">
-        <v>358</v>
+    <row r="5" spans="4:6">
+      <c r="D5" t="s">
+        <v>356</v>
       </c>
       <c r="F5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="5:6">
-      <c r="E6" t="s">
-        <v>359</v>
+    <row r="6" spans="4:6">
+      <c r="D6" t="s">
+        <v>357</v>
       </c>
       <c r="F6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="5:6">
-      <c r="E7" t="s">
-        <v>360</v>
+    <row r="7" spans="4:6">
+      <c r="D7" t="s">
+        <v>358</v>
       </c>
       <c r="F7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="5:6">
-      <c r="E8" t="s">
-        <v>361</v>
+    <row r="8" spans="4:6">
+      <c r="D8" t="s">
+        <v>359</v>
       </c>
       <c r="F8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="5:6">
-      <c r="E9" t="s">
-        <v>362</v>
+    <row r="9" spans="4:6">
+      <c r="D9" t="s">
+        <v>360</v>
       </c>
       <c r="F9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="5:6">
-      <c r="E10" t="s">
-        <v>363</v>
+    <row r="10" spans="4:6">
+      <c r="D10" t="s">
+        <v>361</v>
       </c>
       <c r="F10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="5:6">
-      <c r="E11" t="s">
-        <v>364</v>
+    <row r="11" spans="4:6">
+      <c r="D11" t="s">
+        <v>362</v>
       </c>
       <c r="F11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="5:6">
-      <c r="E12" t="s">
-        <v>365</v>
+    <row r="12" spans="4:6">
+      <c r="D12" t="s">
+        <v>363</v>
       </c>
       <c r="F12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="5:6">
-      <c r="E13" t="s">
+    <row r="13" spans="4:6">
+      <c r="D13" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6">
+      <c r="D14" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6">
+      <c r="D15" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="14" spans="5:6">
-      <c r="E14" t="s">
+    <row r="16" spans="4:6">
+      <c r="D16" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="15" spans="5:6">
-      <c r="E15" t="s">
+    <row r="17" spans="4:4">
+      <c r="D17" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="16" spans="5:6">
-      <c r="E16" t="s">
+    <row r="18" spans="4:4">
+      <c r="D18" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="17" spans="5:5">
-      <c r="E17" t="s">
+    <row r="19" spans="4:4">
+      <c r="D19" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="18" spans="5:5">
-      <c r="E18" t="s">
+    <row r="20" spans="4:4">
+      <c r="D20" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="19" spans="5:5">
-      <c r="E19" t="s">
+    <row r="21" spans="4:4">
+      <c r="D21" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="20" spans="5:5">
-      <c r="E20" t="s">
+    <row r="22" spans="4:4">
+      <c r="D22" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="21" spans="5:5">
-      <c r="E21" t="s">
+    <row r="23" spans="4:4">
+      <c r="D23" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="22" spans="5:5">
-      <c r="E22" t="s">
+    <row r="24" spans="4:4">
+      <c r="D24" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="23" spans="5:5">
-      <c r="E23" t="s">
+    <row r="25" spans="4:4">
+      <c r="D25" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="24" spans="5:5">
-      <c r="E24" t="s">
+    <row r="26" spans="4:4">
+      <c r="D26" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="25" spans="5:5">
-      <c r="E25" t="s">
+    <row r="27" spans="4:4">
+      <c r="D27" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="26" spans="5:5">
-      <c r="E26" t="s">
+    <row r="28" spans="4:4">
+      <c r="D28" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="27" spans="5:5">
-      <c r="E27" t="s">
+    <row r="29" spans="4:4">
+      <c r="D29" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="28" spans="5:5">
-      <c r="E28" t="s">
+    <row r="30" spans="4:4">
+      <c r="D30" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="29" spans="5:5">
-      <c r="E29" t="s">
+    <row r="31" spans="4:4">
+      <c r="D31" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="30" spans="5:5">
-      <c r="E30" t="s">
+    <row r="32" spans="4:4">
+      <c r="D32" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="31" spans="5:5">
-      <c r="E31" t="s">
+    <row r="33" spans="4:4">
+      <c r="D33" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="32" spans="5:5">
-      <c r="E32" t="s">
+    <row r="34" spans="4:4">
+      <c r="D34" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="33" spans="5:5">
-      <c r="E33" t="s">
+    <row r="35" spans="4:4">
+      <c r="D35" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="34" spans="5:5">
-      <c r="E34" t="s">
+    <row r="36" spans="4:4">
+      <c r="D36" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="35" spans="5:5">
-      <c r="E35" t="s">
+    <row r="37" spans="4:4">
+      <c r="D37" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="36" spans="5:5">
-      <c r="E36" t="s">
+    <row r="38" spans="4:4">
+      <c r="D38" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="37" spans="5:5">
-      <c r="E37" t="s">
+    <row r="39" spans="4:4">
+      <c r="D39" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="38" spans="5:5">
-      <c r="E38" t="s">
+    <row r="40" spans="4:4">
+      <c r="D40" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="39" spans="5:5">
-      <c r="E39" t="s">
+    <row r="41" spans="4:4">
+      <c r="D41" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="40" spans="5:5">
-      <c r="E40" t="s">
+    <row r="42" spans="4:4">
+      <c r="D42" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="41" spans="5:5">
-      <c r="E41" t="s">
+    <row r="43" spans="4:4">
+      <c r="D43" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="42" spans="5:5">
-      <c r="E42" t="s">
+    <row r="44" spans="4:4">
+      <c r="D44" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="43" spans="5:5">
-      <c r="E43" t="s">
+    <row r="45" spans="4:4">
+      <c r="D45" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="44" spans="5:5">
-      <c r="E44" t="s">
+    <row r="46" spans="4:4">
+      <c r="D46" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="45" spans="5:5">
-      <c r="E45" t="s">
+    <row r="47" spans="4:4">
+      <c r="D47" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="46" spans="5:5">
-      <c r="E46" t="s">
+    <row r="48" spans="4:4">
+      <c r="D48" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="47" spans="5:5">
-      <c r="E47" t="s">
+    <row r="49" spans="4:4">
+      <c r="D49" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="48" spans="5:5">
-      <c r="E48" t="s">
+    <row r="50" spans="4:4">
+      <c r="D50" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="49" spans="5:5">
-      <c r="E49" t="s">
+    <row r="51" spans="4:4">
+      <c r="D51" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="50" spans="5:5">
-      <c r="E50" t="s">
+    <row r="52" spans="4:4">
+      <c r="D52" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="51" spans="5:5">
-      <c r="E51" t="s">
+    <row r="53" spans="4:4">
+      <c r="D53" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="52" spans="5:5">
-      <c r="E52" t="s">
+    <row r="54" spans="4:4">
+      <c r="D54" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="53" spans="5:5">
-      <c r="E53" t="s">
+    <row r="55" spans="4:4">
+      <c r="D55" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="54" spans="5:5">
-      <c r="E54" t="s">
+    <row r="56" spans="4:4">
+      <c r="D56" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="55" spans="5:5">
-      <c r="E55" t="s">
+    <row r="57" spans="4:4">
+      <c r="D57" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="56" spans="5:5">
-      <c r="E56" t="s">
+    <row r="58" spans="4:4">
+      <c r="D58" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="57" spans="5:5">
-      <c r="E57" t="s">
+    <row r="59" spans="4:4">
+      <c r="D59" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="58" spans="5:5">
-      <c r="E58" t="s">
+    <row r="60" spans="4:4">
+      <c r="D60" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="59" spans="5:5">
-      <c r="E59" t="s">
+    <row r="61" spans="4:4">
+      <c r="D61" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="60" spans="5:5">
-      <c r="E60" t="s">
+    <row r="62" spans="4:4">
+      <c r="D62" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="61" spans="5:5">
-      <c r="E61" t="s">
+    <row r="63" spans="4:4">
+      <c r="D63" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="62" spans="5:5">
-      <c r="E62" t="s">
+    <row r="64" spans="4:4">
+      <c r="D64" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="63" spans="5:5">
-      <c r="E63" t="s">
+    <row r="65" spans="4:4">
+      <c r="D65" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="64" spans="5:5">
-      <c r="E64" t="s">
+    <row r="66" spans="4:4">
+      <c r="D66" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="65" spans="5:5">
-      <c r="E65" t="s">
+    <row r="67" spans="4:4">
+      <c r="D67" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="66" spans="5:5">
-      <c r="E66" t="s">
+    <row r="68" spans="4:4">
+      <c r="D68" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="67" spans="5:5">
-      <c r="E67" t="s">
+    <row r="69" spans="4:4">
+      <c r="D69" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="68" spans="5:5">
-      <c r="E68" t="s">
+    <row r="70" spans="4:4">
+      <c r="D70" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="69" spans="5:5">
-      <c r="E69" t="s">
+    <row r="71" spans="4:4">
+      <c r="D71" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="70" spans="5:5">
-      <c r="E70" t="s">
+    <row r="72" spans="4:4">
+      <c r="D72" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="71" spans="5:5">
-      <c r="E71" t="s">
+    <row r="73" spans="4:4">
+      <c r="D73" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="72" spans="5:5">
-      <c r="E72" t="s">
+    <row r="74" spans="4:4">
+      <c r="D74" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="73" spans="5:5">
-      <c r="E73" t="s">
+    <row r="75" spans="4:4">
+      <c r="D75" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="74" spans="5:5">
-      <c r="E74" t="s">
+    <row r="76" spans="4:4">
+      <c r="D76" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="75" spans="5:5">
-      <c r="E75" t="s">
+    <row r="77" spans="4:4">
+      <c r="D77" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="76" spans="5:5">
-      <c r="E76" t="s">
+    <row r="78" spans="4:4">
+      <c r="D78" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="77" spans="5:5">
-      <c r="E77" t="s">
+    <row r="79" spans="4:4">
+      <c r="D79" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="78" spans="5:5">
-      <c r="E78" t="s">
+    <row r="80" spans="4:4">
+      <c r="D80" t="s">
         <v>431</v>
-      </c>
-    </row>
-    <row r="79" spans="5:5">
-      <c r="E79" t="s">
-        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -4164,7 +4166,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="995B" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="D861" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -4179,88 +4181,88 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BW4"/>
+  <dimension ref="A1:BV4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="54.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="42" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="93.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="183.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="57" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="97.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="64.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="99.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="77.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="57.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="64.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="143.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="79" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="105" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="62.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="70.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="102.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="102.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="91.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="61.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="60.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="67.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="25.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="41.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="121.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="115.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="43.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="52.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="64.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="255.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="77.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="63.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="255.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="76.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="161.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="60.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="61.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="48.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="76.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="77.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="151.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="83.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="101.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="110.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="46.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="62.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="59.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="68.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="124.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="104" style="4" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="41.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="255.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="32.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="129.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="252.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="54.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="80.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="77.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="77.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="255.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="242.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="40" style="4" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="244.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="167" style="4" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="95.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="28.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="86.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="88.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="59.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="255.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="93.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="183.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="57" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="97.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="64.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="99.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="77.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="57.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="64.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="143.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="79" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="105" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="70.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="102.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="102.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="91.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="61.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="60.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="67.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="41.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="121.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="115.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="43.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="52.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="64.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="255.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="77.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="63.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="255.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="76.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="161.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="60.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="61.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="48.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="76.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="77.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="151.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="83.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="101.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="110.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="46.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="62.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="59.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="68.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="124.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="104" style="4" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="41.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="255.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="32.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="129.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="252.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="54.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="80.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="77.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="77.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="255.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="242.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="40" style="4" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="244.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="167" style="4" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="95.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="28.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="86.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="88.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="59.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="255.7109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75">
+    <row r="1" spans="1:74">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -4268,234 +4270,231 @@
         <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="BV1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:74">
+      <c r="A2" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="2" spans="1:75">
-      <c r="A2" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>216</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>216</v>
@@ -4642,7 +4641,7 @@
         <v>310</v>
       </c>
       <c r="AZ2" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="BA2" s="5" t="s">
         <v>313</v>
@@ -4672,7 +4671,7 @@
         <v>329</v>
       </c>
       <c r="BJ2" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="BK2" s="5" t="s">
         <v>332</v>
@@ -4710,19 +4709,16 @@
       <c r="BV2" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="BW2" s="5" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="3" spans="1:75">
+    </row>
+    <row r="3" spans="1:74">
       <c r="A3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>215</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>217</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>217</v>
@@ -4866,10 +4862,10 @@
         <v>309</v>
       </c>
       <c r="AY3" s="5" t="s">
-        <v>311</v>
+        <v>253</v>
       </c>
       <c r="AZ3" s="5" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="BA3" s="5" t="s">
         <v>314</v>
@@ -4896,10 +4892,10 @@
         <v>328</v>
       </c>
       <c r="BI3" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="BJ3" s="5" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="BK3" s="5" t="s">
         <v>333</v>
@@ -4937,11 +4933,8 @@
       <c r="BV3" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="BW3" s="5" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="4" spans="1:75">
+    </row>
+    <row r="4" spans="1:74">
       <c r="A4" s="6" t="s">
         <v>32</v>
       </c>
@@ -5018,29 +5011,28 @@
       <c r="BT4" s="6"/>
       <c r="BU4" s="6"/>
       <c r="BV4" s="6"/>
-      <c r="BW4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="8626" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A613" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
-    <mergeCell ref="A4:BW4"/>
+    <mergeCell ref="A4:BV4"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:BW4">
+  <conditionalFormatting sqref="A1:BV4">
     <cfRule type="notContainsErrors" dxfId="0" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="D5:D1005">
+      <formula1>HiddenDropdowns!$D$5:$D$80</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="E5:E1005">
-      <formula1>HiddenDropdowns!$E$5:$E$79</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="F5:F1005">
       <formula1>"Air Dried,Dry Ice,Ethanol/Dry Ice Slurry,Lyophilised,Not Applicable,Not Collected,Not Provided,Other,Rnalater,Snap Frozen"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="V5:V1005">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="U5:U1005">
       <formula1>"Deaccessioned,Destroyed,In Collection,Missing,On Loan,Used Up"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="AU5:AU1005">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="AT5:AT1005">
       <formula1>"Fruit-Bearing,In Bloom,Non-Reproductive,Pregnant"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5074,34 +5066,34 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>435</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -5109,34 +5101,34 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -5144,34 +5136,34 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -5190,7 +5182,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E801" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="DD20" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -5201,7 +5193,7 @@
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="F5:F1005">
-      <formula1>"10X Nuclei Isolation Kit,3' Standard Throughput Kit"</formula1>
+      <formula1>"10X Nuclei Isolation Kit,3' Standard Throughput Kit,Custom"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5240,40 +5232,40 @@
         <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>471</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>488</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -5281,43 +5273,43 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>504</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>505</v>
-      </c>
       <c r="L2" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="M2" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>509</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -5325,43 +5317,43 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -5383,7 +5375,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="AF32" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A7F1" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -5442,79 +5434,79 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>514</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>548</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="2" spans="1:26">
@@ -5522,79 +5514,79 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>552</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>553</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="Y2" s="5" t="s">
+        <v>594</v>
+      </c>
+      <c r="Z2" s="5" t="s">
         <v>595</v>
-      </c>
-      <c r="Z2" s="5" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -5602,79 +5594,79 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -5708,7 +5700,7 @@
       <c r="Z4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E86C" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="ADC3" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:Z4"/>
   </mergeCells>
@@ -5772,43 +5764,43 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>601</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>614</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>617</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -5816,43 +5808,43 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>631</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>632</v>
-      </c>
       <c r="J2" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>634</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>634</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>635</v>
-      </c>
       <c r="M2" s="5" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -5860,43 +5852,43 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -5918,7 +5910,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="BA84" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="CDD9" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Fixed issue with search functionality where clicking an item would not properly navigate to it on the pag
</commit_message>
<xml_diff>
--- a/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.1.xlsx
+++ b/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.1.xlsx
@@ -2832,7 +2832,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="F054" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="92EC" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2913,7 +2913,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="B0C9" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="87D7" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -3120,7 +3120,7 @@
       <c r="O4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="CD84" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="8DD9" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>
   </mergeCells>
@@ -3196,7 +3196,7 @@
       <c r="D4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="AFE2" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9342" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
   </mergeCells>
@@ -3318,7 +3318,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E6F0" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E91F" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -3504,7 +3504,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="8224" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9BDC" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -3615,7 +3615,7 @@
       <c r="G4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="9288" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="B0B3" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:G4"/>
   </mergeCells>
@@ -4166,7 +4166,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D861" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="C390" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -5013,7 +5013,7 @@
       <c r="BV4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A613" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="F260" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:BV4"/>
   </mergeCells>
@@ -5182,7 +5182,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="DD20" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E7FE" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -5375,7 +5375,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A7F1" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="ED96" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -5700,7 +5700,7 @@
       <c r="Z4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="ADC3" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="B65A" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:Z4"/>
   </mergeCells>
@@ -5910,7 +5910,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="CDD9" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="FB28" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Made content updates dynamic instead of reloading the page; fixed search query issue.
</commit_message>
<xml_diff>
--- a/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.1.xlsx
+++ b/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="912">
   <si>
     <t>key</t>
   </si>
@@ -116,7 +116,7 @@
     <t>The workflow or protocol followed during the study.</t>
   </si>
   <si>
-    <t>e.g. spatial_transcriptomics</t>
+    <t>e.g. Laser microdissection</t>
   </si>
   <si>
     <t>The sorting or visualisation technology used.</t>
@@ -1112,6 +1112,9 @@
     <t>Bodywall</t>
   </si>
   <si>
+    <t>Bone Marrow Hematopoietic Niches</t>
+  </si>
+  <si>
     <t>Bract</t>
   </si>
   <si>
@@ -1127,6 +1130,18 @@
     <t>Cephalothorax</t>
   </si>
   <si>
+    <t>Cortex Development In Roots</t>
+  </si>
+  <si>
+    <t>Developing Brain</t>
+  </si>
+  <si>
+    <t>Developing Embryo</t>
+  </si>
+  <si>
+    <t>Developing Seed Coat</t>
+  </si>
+  <si>
     <t>Dna Extract</t>
   </si>
   <si>
@@ -1136,6 +1151,9 @@
     <t>Eggshell</t>
   </si>
   <si>
+    <t>Embryonic Stem Cells</t>
+  </si>
+  <si>
     <t>Endocrine Tissue</t>
   </si>
   <si>
@@ -1148,12 +1166,30 @@
     <t>Fat Body</t>
   </si>
   <si>
+    <t>Fetal Heart</t>
+  </si>
+  <si>
+    <t>Fetal Kidney</t>
+  </si>
+  <si>
+    <t>Fetal Liver</t>
+  </si>
+  <si>
+    <t>Fetal Lung</t>
+  </si>
+  <si>
     <t>Fin</t>
   </si>
   <si>
+    <t>Floral Meristem</t>
+  </si>
+  <si>
     <t>Flower</t>
   </si>
   <si>
+    <t>Gastrulation-Stage Embryo</t>
+  </si>
+  <si>
     <t>Gill Animal</t>
   </si>
   <si>
@@ -1163,6 +1199,9 @@
     <t>Gonad</t>
   </si>
   <si>
+    <t>Gut</t>
+  </si>
+  <si>
     <t>Hair</t>
   </si>
   <si>
@@ -1178,6 +1217,9 @@
     <t>Holdfast Fungi</t>
   </si>
   <si>
+    <t>Hypocotyl</t>
+  </si>
+  <si>
     <t>Inflorescence</t>
   </si>
   <si>
@@ -1190,9 +1232,15 @@
     <t>Leaf</t>
   </si>
   <si>
+    <t>Leaf Primordia</t>
+  </si>
+  <si>
     <t>Leg</t>
   </si>
   <si>
+    <t>Limb Bud</t>
+  </si>
+  <si>
     <t>Liver</t>
   </si>
   <si>
@@ -1220,6 +1268,15 @@
     <t>Mycorrhiza</t>
   </si>
   <si>
+    <t>Neonatal Retina</t>
+  </si>
+  <si>
+    <t>Neural Crest Cells</t>
+  </si>
+  <si>
+    <t>Nodules</t>
+  </si>
+  <si>
     <t>Not Applicable</t>
   </si>
   <si>
@@ -1229,6 +1286,9 @@
     <t>Not Provided</t>
   </si>
   <si>
+    <t>Olfactory Epithelium</t>
+  </si>
+  <si>
     <t>Other Fungal Tissue</t>
   </si>
   <si>
@@ -1247,18 +1307,36 @@
     <t>Oviduct</t>
   </si>
   <si>
+    <t>Ovule Primordium</t>
+  </si>
+  <si>
     <t>Pancreas</t>
   </si>
   <si>
     <t>Petiole</t>
   </si>
   <si>
+    <t>Placental Trophoblast Cells</t>
+  </si>
+  <si>
+    <t>Pollen Mother Cells</t>
+  </si>
+  <si>
     <t>Posterior Body</t>
   </si>
   <si>
+    <t>Postnatal Thymus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rhizome Meristem </t>
+  </si>
+  <si>
     <t>Root</t>
   </si>
   <si>
+    <t>Root Apical Meristem</t>
+  </si>
+  <si>
     <t>Scales</t>
   </si>
   <si>
@@ -1274,9 +1352,15 @@
     <t>Shoot</t>
   </si>
   <si>
+    <t>Shoot Apical Meristem</t>
+  </si>
+  <si>
     <t>Skin</t>
   </si>
   <si>
+    <t>Somitic Mesoderm</t>
+  </si>
+  <si>
     <t>Sperm Seminal Fluid</t>
   </si>
   <si>
@@ -1316,9 +1400,15 @@
     <t>Thorax</t>
   </si>
   <si>
+    <t>Trichome Precursor Cells</t>
+  </si>
+  <si>
     <t>Unicellular Organisms In Culture</t>
   </si>
   <si>
+    <t>Vascular Cambium</t>
+  </si>
+  <si>
     <t>Whole Organism</t>
   </si>
   <si>
@@ -1538,10 +1628,10 @@
     <t>e.g. 10</t>
   </si>
   <si>
-    <t>The volume of the cell suspension in microlitres.</t>
-  </si>
-  <si>
-    <t>The concentration of cells in the suspension.</t>
+    <t>The volume of the cell suspension in microlitres (µL).</t>
+  </si>
+  <si>
+    <t>The concentration of cells in the suspension in microlitres (µL).</t>
   </si>
   <si>
     <t>e.g. 1000</t>
@@ -1634,6 +1724,9 @@
     <t>cell_phenotype</t>
   </si>
   <si>
+    <t>design_description</t>
+  </si>
+  <si>
     <t>amplification_method (optional)</t>
   </si>
   <si>
@@ -1676,6 +1769,9 @@
     <t>cell_phenotype (optional)</t>
   </si>
   <si>
+    <t>design_description (optional)</t>
+  </si>
+  <si>
     <t>A unique alphanumeric reference or identifier for the library preparation protocol used during the sequencing.</t>
   </si>
   <si>
@@ -1820,6 +1916,12 @@
     <t>e.g. CD41-</t>
   </si>
   <si>
+    <t>The design of the library including details of how it was constructed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e.g. </t>
+  </si>
+  <si>
     <t>sequencing_id</t>
   </si>
   <si>
@@ -1947,6 +2049,255 @@
   </si>
   <si>
     <t>e.g. 75</t>
+  </si>
+  <si>
+    <t>454 Gs</t>
+  </si>
+  <si>
+    <t>454 Gs 20</t>
+  </si>
+  <si>
+    <t>454 Gs Flx</t>
+  </si>
+  <si>
+    <t>454 Gs Flx Titanium</t>
+  </si>
+  <si>
+    <t>454 Gs Flx+</t>
+  </si>
+  <si>
+    <t>454 Gs Junior</t>
+  </si>
+  <si>
+    <t>Ab 310 Genetic Analyzer</t>
+  </si>
+  <si>
+    <t>Ab 3130 Genetic Analyzer</t>
+  </si>
+  <si>
+    <t>Ab 3130Xl Genetic Analyzer</t>
+  </si>
+  <si>
+    <t>Ab 3500 Genetic Analyzer</t>
+  </si>
+  <si>
+    <t>Ab 3500Xl Genetic Analyzer</t>
+  </si>
+  <si>
+    <t>Ab 3730 Genetic Analyzer</t>
+  </si>
+  <si>
+    <t>Ab 3730Xl Genetic Analyzer</t>
+  </si>
+  <si>
+    <t>Ab 5500 Genetic Analyzer</t>
+  </si>
+  <si>
+    <t>Ab 5500Xl Genetic Analyzer</t>
+  </si>
+  <si>
+    <t>Ab 5500Xl-W Genetic Analysis System</t>
+  </si>
+  <si>
+    <t>Ab Solid 3 Plus System</t>
+  </si>
+  <si>
+    <t>Ab Solid 4 System</t>
+  </si>
+  <si>
+    <t>Ab Solid 4Hq System</t>
+  </si>
+  <si>
+    <t>Ab Solid Pi System</t>
+  </si>
+  <si>
+    <t>Ab Solid System</t>
+  </si>
+  <si>
+    <t>Ab Solid System 2.0</t>
+  </si>
+  <si>
+    <t>Ab Solid System 3.0</t>
+  </si>
+  <si>
+    <t>Bgiseq-50</t>
+  </si>
+  <si>
+    <t>Bgiseq-500</t>
+  </si>
+  <si>
+    <t>Complete Genomics</t>
+  </si>
+  <si>
+    <t>Dnbseq-G400</t>
+  </si>
+  <si>
+    <t>Dnbseq-G400 Fast</t>
+  </si>
+  <si>
+    <t>Dnbseq-G50</t>
+  </si>
+  <si>
+    <t>Dnbseq-T10X4Rs</t>
+  </si>
+  <si>
+    <t>Dnbseq-T7</t>
+  </si>
+  <si>
+    <t>Element Aviti</t>
+  </si>
+  <si>
+    <t>Fastaseq 300</t>
+  </si>
+  <si>
+    <t>Genapsys Sequencer</t>
+  </si>
+  <si>
+    <t>Genius</t>
+  </si>
+  <si>
+    <t>Genocare 1600</t>
+  </si>
+  <si>
+    <t>Genolab M</t>
+  </si>
+  <si>
+    <t>Gridion</t>
+  </si>
+  <si>
+    <t>Gs111</t>
+  </si>
+  <si>
+    <t>Illumina Genome Analyzer</t>
+  </si>
+  <si>
+    <t>Illumina Genome Analyzer Ii</t>
+  </si>
+  <si>
+    <t>Illumina Genome Analyzer Iix</t>
+  </si>
+  <si>
+    <t>Illumina Hiscansq</t>
+  </si>
+  <si>
+    <t>Illumina Hiseq 1000</t>
+  </si>
+  <si>
+    <t>Illumina Hiseq 1500</t>
+  </si>
+  <si>
+    <t>Illumina Hiseq 2000</t>
+  </si>
+  <si>
+    <t>Illumina Hiseq 2500</t>
+  </si>
+  <si>
+    <t>Illumina Hiseq 3000</t>
+  </si>
+  <si>
+    <t>Illumina Hiseq 4000</t>
+  </si>
+  <si>
+    <t>Illumina Hiseq X</t>
+  </si>
+  <si>
+    <t>Illumina Hiseq X Five</t>
+  </si>
+  <si>
+    <t>Illumina Hiseq X Ten</t>
+  </si>
+  <si>
+    <t>Illumina Iseq 100</t>
+  </si>
+  <si>
+    <t>Illumina Miniseq</t>
+  </si>
+  <si>
+    <t>Illumina Miseq</t>
+  </si>
+  <si>
+    <t>Illumina Nextseq 500</t>
+  </si>
+  <si>
+    <t>Illumina Nextseq 550</t>
+  </si>
+  <si>
+    <t>Illumina Novaseq 6000</t>
+  </si>
+  <si>
+    <t>Illumina Novaseq X</t>
+  </si>
+  <si>
+    <t>Illumina Novaseq X Plus</t>
+  </si>
+  <si>
+    <t>Ion Genestudio S5</t>
+  </si>
+  <si>
+    <t>Ion Genestudio S5 Plus</t>
+  </si>
+  <si>
+    <t>Ion Genestudio S5 Prime</t>
+  </si>
+  <si>
+    <t>Ion Torrent Genexus</t>
+  </si>
+  <si>
+    <t>Ion Torrent Pgm</t>
+  </si>
+  <si>
+    <t>Ion Torrent Proton</t>
+  </si>
+  <si>
+    <t>Ion Torrent S5</t>
+  </si>
+  <si>
+    <t>Ion Torrent S5 Xl</t>
+  </si>
+  <si>
+    <t>Mgiseq-2000Rs</t>
+  </si>
+  <si>
+    <t>Minion</t>
+  </si>
+  <si>
+    <t>Nextseq 1000</t>
+  </si>
+  <si>
+    <t>Nextseq 2000</t>
+  </si>
+  <si>
+    <t>Onso</t>
+  </si>
+  <si>
+    <t>Pacbio Rs</t>
+  </si>
+  <si>
+    <t>Pacbio Rs Ii</t>
+  </si>
+  <si>
+    <t>Promethion</t>
+  </si>
+  <si>
+    <t>Revio</t>
+  </si>
+  <si>
+    <t>Sentosa Sq301</t>
+  </si>
+  <si>
+    <t>Sequel</t>
+  </si>
+  <si>
+    <t>Sequel Ii</t>
+  </si>
+  <si>
+    <t>Sequel Iie</t>
+  </si>
+  <si>
+    <t>Tapestri</t>
+  </si>
+  <si>
+    <t>Ug 100</t>
   </si>
   <si>
     <t>file_derived_from</t>
@@ -2307,10 +2658,16 @@
     <t>index_2_file</t>
   </si>
   <si>
-    <t>read_checksum</t>
-  </si>
-  <si>
-    <t>index_checksum</t>
+    <t>read_1_checksum</t>
+  </si>
+  <si>
+    <t>read_2_checksum</t>
+  </si>
+  <si>
+    <t>index_1_checksum</t>
+  </si>
+  <si>
+    <t>index_2_checksum</t>
   </si>
   <si>
     <t>white_list_barcode_file</t>
@@ -2325,6 +2682,18 @@
     <t>expression_data_file</t>
   </si>
   <si>
+    <t>read_2_file (optional)</t>
+  </si>
+  <si>
+    <t>index_1_file (optional)</t>
+  </si>
+  <si>
+    <t>read_2_checksum (optional)</t>
+  </si>
+  <si>
+    <t>index_2_checksum (optional)</t>
+  </si>
+  <si>
     <t>white_list_barcode_file (optional)</t>
   </si>
   <si>
@@ -2358,16 +2727,19 @@
     <t>e.g. file2_i2.fastq.gz</t>
   </si>
   <si>
-    <t>Result of a hash function calculated on the content of both the read 1 file and the read 2 file to verify file integrity. Commonly used algorithms include MD5 and SHA-1. The checksums should be separated by a comma (,).</t>
-  </si>
-  <si>
-    <t>e.g. d41d8cd98f00b204e9800998ecf8427e,5a105e8b9d40e1329780d62ea2265d8a77a1a45e</t>
-  </si>
-  <si>
-    <t>Result of a hash function calculated on the content of both the index 1 file and the index 2 file to verify file integrity. Commonly used algorithms include MD5 and SHA-1. The checksums should be separated by a comma (,).</t>
-  </si>
-  <si>
-    <t>e.g. d3486ae9136e7856bc42212385ea797094475802,b7e23ec29af22b0b4e41da31e868d57226121c84</t>
+    <t>Result of a hash function calculated on the content of the read 1 file  to verify file integrity. Commonly used algorithms include MD5 and SHA-1. The checksums should be separated by a comma (,).</t>
+  </si>
+  <si>
+    <t>e.g. d41d8cd98f00b204e9800998ecf8427e</t>
+  </si>
+  <si>
+    <t>Result of a hash function calculated on the content of the read 2 file  to verify file integrity. Commonly used algorithms include MD5 and SHA-1. The checksums should be separated by a comma (,).</t>
+  </si>
+  <si>
+    <t>Result of a hash function calculated on the content of  the index 1 file  to verify file integrity. Commonly used algorithms include MD5 and SHA-1. The checksums should be separated by a comma (,).</t>
+  </si>
+  <si>
+    <t>Result of a hash function calculated on the content of  the index 2 file  to verify file integrity. Commonly used algorithms include MD5 and SHA-1. The checksums should be separated by a comma (,).</t>
   </si>
   <si>
     <t>A file containing the known cell barcodes in the
@@ -2832,7 +3204,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="92EC" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="DE85" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2857,16 +3229,16 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>644</v>
+        <v>761</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>645</v>
+        <v>762</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>646</v>
+        <v>763</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>647</v>
+        <v>764</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2874,16 +3246,16 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>648</v>
+        <v>765</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>650</v>
+        <v>767</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>652</v>
+        <v>769</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>654</v>
+        <v>771</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2891,16 +3263,16 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>649</v>
+        <v>766</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>651</v>
+        <v>768</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>653</v>
+        <v>770</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>655</v>
+        <v>772</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2913,7 +3285,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="87D7" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="F306" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -2964,46 +3336,46 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>670</v>
+        <v>787</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>671</v>
+        <v>788</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>672</v>
+        <v>789</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>673</v>
+        <v>790</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>674</v>
+        <v>791</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>675</v>
+        <v>792</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>676</v>
+        <v>793</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>677</v>
+        <v>794</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>678</v>
+        <v>795</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>679</v>
+        <v>796</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>680</v>
+        <v>797</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>681</v>
+        <v>798</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>682</v>
+        <v>799</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>683</v>
+        <v>800</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -3011,46 +3383,46 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>684</v>
+        <v>801</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>686</v>
+        <v>803</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>688</v>
+        <v>805</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>690</v>
+        <v>807</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>692</v>
+        <v>809</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>694</v>
+        <v>811</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>696</v>
+        <v>813</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>698</v>
+        <v>815</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>700</v>
+        <v>817</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>702</v>
+        <v>819</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>704</v>
+        <v>821</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>706</v>
+        <v>823</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>698</v>
+        <v>815</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>709</v>
+        <v>826</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -3058,46 +3430,46 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>685</v>
+        <v>802</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>687</v>
+        <v>804</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>689</v>
+        <v>806</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>691</v>
+        <v>808</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>693</v>
+        <v>810</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>695</v>
+        <v>812</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>697</v>
+        <v>814</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>699</v>
+        <v>816</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>701</v>
+        <v>818</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>703</v>
+        <v>820</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>705</v>
+        <v>822</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>707</v>
+        <v>824</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>708</v>
+        <v>825</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>710</v>
+        <v>827</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -3120,7 +3492,7 @@
       <c r="O4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="8DD9" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="D87B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>
   </mergeCells>
@@ -3150,13 +3522,13 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>714</v>
+        <v>831</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>715</v>
+        <v>832</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>716</v>
+        <v>833</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3164,13 +3536,13 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>717</v>
+        <v>834</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>717</v>
+        <v>834</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>717</v>
+        <v>834</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3178,13 +3550,13 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>718</v>
+        <v>835</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>719</v>
+        <v>836</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>720</v>
+        <v>837</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3196,7 +3568,7 @@
       <c r="D4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="9342" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A611" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
   </mergeCells>
@@ -3229,80 +3601,80 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>729</v>
+        <v>846</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>730</v>
+        <v>847</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>731</v>
+        <v>848</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>732</v>
+        <v>849</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>733</v>
+        <v>850</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>734</v>
+        <v>851</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>735</v>
+        <v>852</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>736</v>
+        <v>853</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>737</v>
+        <v>854</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>739</v>
+        <v>856</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>741</v>
+        <v>858</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>743</v>
+        <v>860</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>745</v>
+        <v>862</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>747</v>
+        <v>864</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>749</v>
+        <v>866</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>751</v>
+        <v>868</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
-        <v>738</v>
+        <v>855</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>740</v>
+        <v>857</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>742</v>
+        <v>859</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>744</v>
+        <v>861</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>746</v>
+        <v>863</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>748</v>
+        <v>865</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>750</v>
+        <v>867</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>752</v>
+        <v>869</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3318,7 +3690,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E91F" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="CBD4" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -3333,7 +3705,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3345,147 +3717,165 @@
     <col min="4" max="4" width="40.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="48.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="49.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="193.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="195.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="80.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="95.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="126.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="172.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="174.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="80.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="95.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="126.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>753</v>
+        <v>870</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>597</v>
+        <v>631</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>754</v>
+        <v>871</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>755</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>756</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>757</v>
+        <v>872</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>885</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>758</v>
+        <v>875</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>759</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>760</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>765</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+        <v>876</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>882</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>549</v>
+        <v>581</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>618</v>
+        <v>652</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>767</v>
+        <v>890</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>768</v>
+        <v>891</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>770</v>
+        <v>893</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>772</v>
+        <v>895</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>774</v>
+        <v>897</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>776</v>
+        <v>899</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>778</v>
+        <v>901</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>780</v>
+        <v>902</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>782</v>
+        <v>903</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>784</v>
+        <v>904</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>906</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>908</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>550</v>
+        <v>582</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>619</v>
+        <v>653</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>769</v>
+        <v>892</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>771</v>
+        <v>894</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>773</v>
+        <v>896</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>775</v>
+        <v>898</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>777</v>
+        <v>900</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>779</v>
+        <v>900</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>781</v>
+        <v>900</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>783</v>
+        <v>900</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>785</v>
+        <v>905</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>907</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>909</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="6" t="s">
         <v>32</v>
       </c>
@@ -3502,13 +3892,15 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="9BDC" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="D1F3" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
-    <mergeCell ref="A4:N4"/>
+    <mergeCell ref="A4:P4"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:N4">
+  <conditionalFormatting sqref="A1:P4">
     <cfRule type="notContainsErrors" dxfId="0" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
@@ -3615,7 +4007,7 @@
       <c r="G4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="B0B3" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="FEE4" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:G4"/>
   </mergeCells>
@@ -3624,12 +4016,9 @@
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="F5:F1005">
       <formula1>HiddenDropdowns!$F$5:$F$12</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="G5:G1005">
-      <formula1>"10X,10X 3',Mas Seq,Smartseq,Vizgen"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3638,19 +4027,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D5:F80"/>
+  <dimension ref="D5:F110"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="4:6">
       <c r="D5" t="s">
-        <v>356</v>
+        <v>674</v>
       </c>
       <c r="F5" t="s">
         <v>33</v>
@@ -3658,7 +4047,7 @@
     </row>
     <row r="6" spans="4:6">
       <c r="D6" t="s">
-        <v>357</v>
+        <v>675</v>
       </c>
       <c r="F6" t="s">
         <v>34</v>
@@ -3666,7 +4055,7 @@
     </row>
     <row r="7" spans="4:6">
       <c r="D7" t="s">
-        <v>358</v>
+        <v>676</v>
       </c>
       <c r="F7" t="s">
         <v>35</v>
@@ -3674,7 +4063,7 @@
     </row>
     <row r="8" spans="4:6">
       <c r="D8" t="s">
-        <v>359</v>
+        <v>677</v>
       </c>
       <c r="F8" t="s">
         <v>36</v>
@@ -3682,7 +4071,7 @@
     </row>
     <row r="9" spans="4:6">
       <c r="D9" t="s">
-        <v>360</v>
+        <v>678</v>
       </c>
       <c r="F9" t="s">
         <v>37</v>
@@ -3690,7 +4079,7 @@
     </row>
     <row r="10" spans="4:6">
       <c r="D10" t="s">
-        <v>361</v>
+        <v>679</v>
       </c>
       <c r="F10" t="s">
         <v>38</v>
@@ -3698,7 +4087,7 @@
     </row>
     <row r="11" spans="4:6">
       <c r="D11" t="s">
-        <v>362</v>
+        <v>680</v>
       </c>
       <c r="F11" t="s">
         <v>39</v>
@@ -3706,7 +4095,7 @@
     </row>
     <row r="12" spans="4:6">
       <c r="D12" t="s">
-        <v>363</v>
+        <v>681</v>
       </c>
       <c r="F12" t="s">
         <v>40</v>
@@ -3714,342 +4103,492 @@
     </row>
     <row r="13" spans="4:6">
       <c r="D13" t="s">
-        <v>364</v>
+        <v>682</v>
       </c>
     </row>
     <row r="14" spans="4:6">
       <c r="D14" t="s">
-        <v>365</v>
+        <v>683</v>
       </c>
     </row>
     <row r="15" spans="4:6">
       <c r="D15" t="s">
-        <v>366</v>
+        <v>684</v>
       </c>
     </row>
     <row r="16" spans="4:6">
       <c r="D16" t="s">
-        <v>367</v>
+        <v>685</v>
       </c>
     </row>
     <row r="17" spans="4:4">
       <c r="D17" t="s">
-        <v>368</v>
+        <v>686</v>
       </c>
     </row>
     <row r="18" spans="4:4">
       <c r="D18" t="s">
-        <v>369</v>
+        <v>687</v>
       </c>
     </row>
     <row r="19" spans="4:4">
       <c r="D19" t="s">
-        <v>370</v>
+        <v>688</v>
       </c>
     </row>
     <row r="20" spans="4:4">
       <c r="D20" t="s">
-        <v>371</v>
+        <v>689</v>
       </c>
     </row>
     <row r="21" spans="4:4">
       <c r="D21" t="s">
-        <v>372</v>
+        <v>690</v>
       </c>
     </row>
     <row r="22" spans="4:4">
       <c r="D22" t="s">
-        <v>373</v>
+        <v>691</v>
       </c>
     </row>
     <row r="23" spans="4:4">
       <c r="D23" t="s">
-        <v>374</v>
+        <v>692</v>
       </c>
     </row>
     <row r="24" spans="4:4">
       <c r="D24" t="s">
-        <v>375</v>
+        <v>693</v>
       </c>
     </row>
     <row r="25" spans="4:4">
       <c r="D25" t="s">
-        <v>376</v>
+        <v>694</v>
       </c>
     </row>
     <row r="26" spans="4:4">
       <c r="D26" t="s">
-        <v>377</v>
+        <v>695</v>
       </c>
     </row>
     <row r="27" spans="4:4">
       <c r="D27" t="s">
-        <v>378</v>
+        <v>696</v>
       </c>
     </row>
     <row r="28" spans="4:4">
       <c r="D28" t="s">
-        <v>379</v>
+        <v>697</v>
       </c>
     </row>
     <row r="29" spans="4:4">
       <c r="D29" t="s">
-        <v>380</v>
+        <v>698</v>
       </c>
     </row>
     <row r="30" spans="4:4">
       <c r="D30" t="s">
-        <v>381</v>
+        <v>699</v>
       </c>
     </row>
     <row r="31" spans="4:4">
       <c r="D31" t="s">
-        <v>382</v>
+        <v>700</v>
       </c>
     </row>
     <row r="32" spans="4:4">
       <c r="D32" t="s">
-        <v>383</v>
+        <v>701</v>
       </c>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" t="s">
-        <v>384</v>
+        <v>702</v>
       </c>
     </row>
     <row r="34" spans="4:4">
       <c r="D34" t="s">
-        <v>385</v>
+        <v>703</v>
       </c>
     </row>
     <row r="35" spans="4:4">
       <c r="D35" t="s">
-        <v>386</v>
+        <v>704</v>
       </c>
     </row>
     <row r="36" spans="4:4">
       <c r="D36" t="s">
-        <v>387</v>
+        <v>705</v>
       </c>
     </row>
     <row r="37" spans="4:4">
       <c r="D37" t="s">
-        <v>388</v>
+        <v>706</v>
       </c>
     </row>
     <row r="38" spans="4:4">
       <c r="D38" t="s">
-        <v>389</v>
+        <v>707</v>
       </c>
     </row>
     <row r="39" spans="4:4">
       <c r="D39" t="s">
-        <v>390</v>
+        <v>708</v>
       </c>
     </row>
     <row r="40" spans="4:4">
       <c r="D40" t="s">
-        <v>391</v>
+        <v>709</v>
       </c>
     </row>
     <row r="41" spans="4:4">
       <c r="D41" t="s">
-        <v>392</v>
+        <v>710</v>
       </c>
     </row>
     <row r="42" spans="4:4">
       <c r="D42" t="s">
-        <v>393</v>
+        <v>711</v>
       </c>
     </row>
     <row r="43" spans="4:4">
       <c r="D43" t="s">
-        <v>394</v>
+        <v>712</v>
       </c>
     </row>
     <row r="44" spans="4:4">
       <c r="D44" t="s">
-        <v>395</v>
+        <v>713</v>
       </c>
     </row>
     <row r="45" spans="4:4">
       <c r="D45" t="s">
-        <v>396</v>
+        <v>714</v>
       </c>
     </row>
     <row r="46" spans="4:4">
       <c r="D46" t="s">
-        <v>397</v>
+        <v>715</v>
       </c>
     </row>
     <row r="47" spans="4:4">
       <c r="D47" t="s">
-        <v>398</v>
+        <v>716</v>
       </c>
     </row>
     <row r="48" spans="4:4">
       <c r="D48" t="s">
-        <v>399</v>
+        <v>717</v>
       </c>
     </row>
     <row r="49" spans="4:4">
       <c r="D49" t="s">
-        <v>400</v>
+        <v>718</v>
       </c>
     </row>
     <row r="50" spans="4:4">
       <c r="D50" t="s">
-        <v>401</v>
+        <v>719</v>
       </c>
     </row>
     <row r="51" spans="4:4">
       <c r="D51" t="s">
-        <v>402</v>
+        <v>720</v>
       </c>
     </row>
     <row r="52" spans="4:4">
       <c r="D52" t="s">
-        <v>403</v>
+        <v>721</v>
       </c>
     </row>
     <row r="53" spans="4:4">
       <c r="D53" t="s">
-        <v>404</v>
+        <v>722</v>
       </c>
     </row>
     <row r="54" spans="4:4">
       <c r="D54" t="s">
-        <v>405</v>
+        <v>723</v>
       </c>
     </row>
     <row r="55" spans="4:4">
       <c r="D55" t="s">
-        <v>406</v>
+        <v>724</v>
       </c>
     </row>
     <row r="56" spans="4:4">
       <c r="D56" t="s">
-        <v>407</v>
+        <v>725</v>
       </c>
     </row>
     <row r="57" spans="4:4">
       <c r="D57" t="s">
-        <v>408</v>
+        <v>726</v>
       </c>
     </row>
     <row r="58" spans="4:4">
       <c r="D58" t="s">
-        <v>409</v>
+        <v>727</v>
       </c>
     </row>
     <row r="59" spans="4:4">
       <c r="D59" t="s">
-        <v>410</v>
+        <v>728</v>
       </c>
     </row>
     <row r="60" spans="4:4">
       <c r="D60" t="s">
-        <v>411</v>
+        <v>729</v>
       </c>
     </row>
     <row r="61" spans="4:4">
       <c r="D61" t="s">
-        <v>412</v>
+        <v>730</v>
       </c>
     </row>
     <row r="62" spans="4:4">
       <c r="D62" t="s">
-        <v>413</v>
+        <v>731</v>
       </c>
     </row>
     <row r="63" spans="4:4">
       <c r="D63" t="s">
-        <v>414</v>
+        <v>732</v>
       </c>
     </row>
     <row r="64" spans="4:4">
       <c r="D64" t="s">
-        <v>415</v>
+        <v>733</v>
       </c>
     </row>
     <row r="65" spans="4:4">
       <c r="D65" t="s">
-        <v>416</v>
+        <v>734</v>
       </c>
     </row>
     <row r="66" spans="4:4">
       <c r="D66" t="s">
-        <v>417</v>
+        <v>735</v>
       </c>
     </row>
     <row r="67" spans="4:4">
       <c r="D67" t="s">
-        <v>418</v>
+        <v>736</v>
       </c>
     </row>
     <row r="68" spans="4:4">
       <c r="D68" t="s">
-        <v>419</v>
+        <v>737</v>
       </c>
     </row>
     <row r="69" spans="4:4">
       <c r="D69" t="s">
-        <v>420</v>
+        <v>738</v>
       </c>
     </row>
     <row r="70" spans="4:4">
       <c r="D70" t="s">
-        <v>421</v>
+        <v>739</v>
       </c>
     </row>
     <row r="71" spans="4:4">
       <c r="D71" t="s">
-        <v>422</v>
+        <v>740</v>
       </c>
     </row>
     <row r="72" spans="4:4">
       <c r="D72" t="s">
-        <v>423</v>
+        <v>741</v>
       </c>
     </row>
     <row r="73" spans="4:4">
       <c r="D73" t="s">
-        <v>424</v>
+        <v>742</v>
       </c>
     </row>
     <row r="74" spans="4:4">
       <c r="D74" t="s">
-        <v>425</v>
+        <v>743</v>
       </c>
     </row>
     <row r="75" spans="4:4">
       <c r="D75" t="s">
-        <v>426</v>
+        <v>744</v>
       </c>
     </row>
     <row r="76" spans="4:4">
       <c r="D76" t="s">
-        <v>427</v>
+        <v>745</v>
       </c>
     </row>
     <row r="77" spans="4:4">
       <c r="D77" t="s">
-        <v>428</v>
+        <v>746</v>
       </c>
     </row>
     <row r="78" spans="4:4">
       <c r="D78" t="s">
-        <v>429</v>
+        <v>747</v>
       </c>
     </row>
     <row r="79" spans="4:4">
       <c r="D79" t="s">
-        <v>430</v>
+        <v>748</v>
       </c>
     </row>
     <row r="80" spans="4:4">
       <c r="D80" t="s">
-        <v>431</v>
+        <v>749</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4">
+      <c r="D81" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="82" spans="4:4">
+      <c r="D82" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="83" spans="4:4">
+      <c r="D83" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4">
+      <c r="D84" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="85" spans="4:4">
+      <c r="D85" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="86" spans="4:4">
+      <c r="D86" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="87" spans="4:4">
+      <c r="D87" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="88" spans="4:4">
+      <c r="D88" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="89" spans="4:4">
+      <c r="D89" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="90" spans="4:4">
+      <c r="D90" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="91" spans="4:4">
+      <c r="D91" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="92" spans="4:4">
+      <c r="D92" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="93" spans="4:4">
+      <c r="D93" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="94" spans="4:4">
+      <c r="D94" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="95" spans="4:4">
+      <c r="D95" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="96" spans="4:4">
+      <c r="D96" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4">
+      <c r="D97" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="98" spans="4:4">
+      <c r="D98" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="99" spans="4:4">
+      <c r="D99" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="100" spans="4:4">
+      <c r="D100" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="101" spans="4:4">
+      <c r="D101" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="102" spans="4:4">
+      <c r="D102" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="103" spans="4:4">
+      <c r="D103" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="104" spans="4:4">
+      <c r="D104" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="105" spans="4:4">
+      <c r="D105" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="106" spans="4:4">
+      <c r="D106" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="107" spans="4:4">
+      <c r="D107" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="108" spans="4:4">
+      <c r="D108" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="109" spans="4:4">
+      <c r="D109" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="110" spans="4:4">
+      <c r="D110" t="s">
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -4166,7 +4705,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="C390" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="C503" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -5013,7 +5552,7 @@
       <c r="BV4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="F260" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="B42B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:BV4"/>
   </mergeCells>
@@ -5024,7 +5563,7 @@
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="D5:D1005">
-      <formula1>HiddenDropdowns!$D$5:$D$80</formula1>
+      <formula1>HiddenDropdowns!$D$5:$D$110</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="E5:E1005">
       <formula1>"Air Dried,Dry Ice,Ethanol/Dry Ice Slurry,Lyophilised,Not Applicable,Not Collected,Not Provided,Other,Rnalater,Snap Frozen"</formula1>
@@ -5066,34 +5605,34 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>432</v>
+        <v>462</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>433</v>
+        <v>463</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>434</v>
+        <v>464</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>442</v>
+        <v>472</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>443</v>
+        <v>473</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>444</v>
+        <v>474</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>445</v>
+        <v>475</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>446</v>
+        <v>476</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>447</v>
+        <v>477</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>448</v>
+        <v>478</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -5101,34 +5640,34 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>449</v>
+        <v>479</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>451</v>
+        <v>481</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>453</v>
+        <v>483</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>455</v>
+        <v>485</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>457</v>
+        <v>487</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>459</v>
+        <v>489</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>461</v>
+        <v>491</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>463</v>
+        <v>493</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>465</v>
+        <v>495</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>467</v>
+        <v>497</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -5136,34 +5675,34 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>450</v>
+        <v>480</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>452</v>
+        <v>482</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>454</v>
+        <v>484</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>456</v>
+        <v>486</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>458</v>
+        <v>488</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>460</v>
+        <v>490</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>462</v>
+        <v>492</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>464</v>
+        <v>494</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>466</v>
+        <v>496</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>468</v>
+        <v>498</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -5182,7 +5721,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E7FE" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="DD96" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -5217,8 +5756,8 @@
     <col min="7" max="7" width="99.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="105.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="49.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="45.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="47.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="56.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="37.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="87.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="182.42578125" style="4" bestFit="1" customWidth="1"/>
@@ -5232,40 +5771,40 @@
         <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>432</v>
+        <v>462</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>469</v>
+        <v>499</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>470</v>
+        <v>500</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>480</v>
+        <v>510</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>481</v>
+        <v>511</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>482</v>
+        <v>512</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>483</v>
+        <v>513</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>484</v>
+        <v>514</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>485</v>
+        <v>515</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>486</v>
+        <v>516</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>487</v>
+        <v>517</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>488</v>
+        <v>518</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -5273,43 +5812,43 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>489</v>
+        <v>519</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>449</v>
+        <v>479</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>491</v>
+        <v>521</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>493</v>
+        <v>523</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>495</v>
+        <v>525</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>497</v>
+        <v>527</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>499</v>
+        <v>529</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>501</v>
+        <v>531</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>503</v>
+        <v>533</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>504</v>
+        <v>534</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>506</v>
+        <v>536</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>508</v>
+        <v>538</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>509</v>
+        <v>539</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -5317,43 +5856,43 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>490</v>
+        <v>520</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>450</v>
+        <v>480</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>492</v>
+        <v>522</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>494</v>
+        <v>524</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>496</v>
+        <v>526</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>498</v>
+        <v>528</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>500</v>
+        <v>530</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>502</v>
+        <v>532</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>281</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>505</v>
+        <v>535</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>507</v>
+        <v>537</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>502</v>
+        <v>532</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>510</v>
+        <v>540</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -5375,7 +5914,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="ED96" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="FA2F" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -5395,7 +5934,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5427,249 +5966,259 @@
     <col min="24" max="24" width="61.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="64.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="66.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="61" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>511</v>
+        <v>541</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>469</v>
+        <v>499</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>512</v>
+        <v>542</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>513</v>
+        <v>543</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>535</v>
+        <v>566</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>536</v>
+        <v>567</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>537</v>
+        <v>568</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>538</v>
+        <v>569</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>539</v>
+        <v>570</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>540</v>
+        <v>571</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>520</v>
+        <v>550</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>541</v>
+        <v>572</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>542</v>
+        <v>573</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>523</v>
+        <v>553</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>543</v>
+        <v>574</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>544</v>
+        <v>575</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>526</v>
+        <v>556</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>527</v>
+        <v>557</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>528</v>
+        <v>558</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>529</v>
+        <v>559</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>530</v>
+        <v>560</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>545</v>
+        <v>576</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>546</v>
+        <v>577</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>547</v>
+        <v>578</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26">
+        <v>579</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>549</v>
+        <v>581</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>551</v>
+        <v>583</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>552</v>
+        <v>584</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>554</v>
+        <v>586</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>556</v>
+        <v>588</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>558</v>
+        <v>590</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>560</v>
+        <v>592</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>562</v>
+        <v>594</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>564</v>
+        <v>596</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>566</v>
+        <v>598</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>568</v>
+        <v>600</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>570</v>
+        <v>602</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>572</v>
+        <v>604</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>574</v>
+        <v>606</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>576</v>
+        <v>608</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>578</v>
+        <v>610</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>580</v>
+        <v>612</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>582</v>
+        <v>614</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>584</v>
+        <v>616</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>586</v>
+        <v>618</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>588</v>
+        <v>620</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>590</v>
+        <v>622</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>592</v>
+        <v>624</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>594</v>
+        <v>626</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26">
+        <v>627</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
       <c r="A3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>550</v>
+        <v>582</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>492</v>
+        <v>522</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>553</v>
+        <v>585</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>555</v>
+        <v>587</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>557</v>
+        <v>589</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>559</v>
+        <v>591</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>561</v>
+        <v>593</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>563</v>
+        <v>595</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>565</v>
+        <v>597</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>567</v>
+        <v>599</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>569</v>
+        <v>601</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>571</v>
+        <v>603</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>573</v>
+        <v>605</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>575</v>
+        <v>607</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>577</v>
+        <v>609</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>579</v>
+        <v>611</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>581</v>
+        <v>613</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>583</v>
+        <v>615</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>585</v>
+        <v>617</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>587</v>
+        <v>619</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>589</v>
+        <v>621</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>591</v>
+        <v>623</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>593</v>
+        <v>625</v>
       </c>
       <c r="Y3" s="5" t="s">
         <v>305</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26">
+        <v>628</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
       <c r="A4" s="6" t="s">
         <v>32</v>
       </c>
@@ -5698,13 +6247,14 @@
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="B65A" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E485" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
-    <mergeCell ref="A4:Z4"/>
+    <mergeCell ref="A4:AA4"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:Z4">
+  <conditionalFormatting sqref="A1:AA4">
     <cfRule type="notContainsErrors" dxfId="0" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
@@ -5764,43 +6314,43 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>597</v>
+        <v>631</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>598</v>
+        <v>632</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>599</v>
+        <v>633</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>600</v>
+        <v>634</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>610</v>
+        <v>644</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>611</v>
+        <v>645</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>612</v>
+        <v>646</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>613</v>
+        <v>647</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>614</v>
+        <v>648</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>615</v>
+        <v>649</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>607</v>
+        <v>641</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>616</v>
+        <v>650</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>617</v>
+        <v>651</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -5808,43 +6358,43 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>618</v>
+        <v>652</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>620</v>
+        <v>654</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>622</v>
+        <v>656</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>624</v>
+        <v>658</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>626</v>
+        <v>660</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>628</v>
+        <v>662</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>630</v>
+        <v>664</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>631</v>
+        <v>665</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>633</v>
+        <v>667</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>633</v>
+        <v>667</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>634</v>
+        <v>668</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>636</v>
+        <v>670</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>638</v>
+        <v>672</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -5852,43 +6402,43 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>619</v>
+        <v>653</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>621</v>
+        <v>655</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>623</v>
+        <v>657</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>625</v>
+        <v>659</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>627</v>
+        <v>661</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>629</v>
+        <v>663</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>502</v>
+        <v>532</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>632</v>
+        <v>666</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>502</v>
+        <v>532</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>629</v>
+        <v>663</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>635</v>
+        <v>669</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>637</v>
+        <v>671</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>639</v>
+        <v>673</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -5910,7 +6460,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="FB28" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A2FD" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -5919,7 +6469,10 @@
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="D5:D1005">
+      <formula1>HiddenDropdowns!$D$5:$D$87</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="E5:E1005">
       <formula1>"Other,Paired,Single,Vector"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Updated single cell manifest and outputs
</commit_message>
<xml_diff>
--- a/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.1.xlsx
+++ b/dist/checklists/xlsx/dwc/sc_rnaseq_dwc_v0.1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="912">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="911">
   <si>
     <t>key</t>
   </si>
@@ -2638,9 +2638,6 @@
   </si>
   <si>
     <t>e.g. Barcode information used in multiplexing protocols is provided in a separate file, which can be accessed at: https://example.com/barcode_data.csv.</t>
-  </si>
-  <si>
-    <t>lib_prep_id</t>
   </si>
   <si>
     <t>file_id</t>
@@ -3204,7 +3201,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="FB07" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="C6A8" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3285,7 +3282,7 @@
       <c r="E4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="CDD3" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="B36E" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -3492,7 +3489,7 @@
       <c r="O4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="BEF6" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="8DF2" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>
   </mergeCells>
@@ -3568,7 +3565,7 @@
       <c r="D4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="E001" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="AE38" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
   </mergeCells>
@@ -3690,7 +3687,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="DDC4" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="C412" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -3730,49 +3727,49 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>870</v>
+        <v>541</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>631</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>871</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>872</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>884</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="2" t="s">
+        <v>874</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>885</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>875</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>876</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>886</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>878</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>888</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>881</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>882</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>889</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -3786,43 +3783,43 @@
         <v>652</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>889</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>890</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>891</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>900</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>901</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>902</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>903</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>904</v>
-      </c>
       <c r="N2" s="5" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -3839,40 +3836,40 @@
         <v>19</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -3896,7 +3893,7 @@
       <c r="P4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="D0F2" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="F611" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:P4"/>
   </mergeCells>
@@ -4007,7 +4004,7 @@
       <c r="G4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="CF20" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="F0E6" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:G4"/>
   </mergeCells>
@@ -4705,7 +4702,7 @@
       <c r="H4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="FCF5" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="B63F" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:H4"/>
   </mergeCells>
@@ -5552,7 +5549,7 @@
       <c r="BV4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="B6D8" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="E660" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:BV4"/>
   </mergeCells>
@@ -5721,7 +5718,7 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="9A4A" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9933" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:K4"/>
   </mergeCells>
@@ -5914,7 +5911,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="C434" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="AE0C" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>
@@ -6250,7 +6247,7 @@
       <c r="AA4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="8EBE" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="8AD1" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:AA4"/>
   </mergeCells>
@@ -6460,7 +6457,7 @@
       <c r="N4" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection password="A461" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="DB3E" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A4:N4"/>
   </mergeCells>

</xml_diff>